<commit_message>
lecture 4 report almost done
</commit_message>
<xml_diff>
--- a/dist_test.xlsx
+++ b/dist_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Videos\Studia\Quant Suisse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scripts\quant_suisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{199953AE-9B68-4636-A7A7-B37EAB6AFBB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F224AB59-179E-4A79-965C-DCA46B80B678}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dist_test" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,15 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">dist_test!$A$1:$ALL$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">dist_test!$A$1:$ALL$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">dist_test!$A$1:$ALL$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">dist_test!$A$1:$ALL$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -524,8 +522,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -589,12 +588,39 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.1</cx:f>
+        <cx:f dir="row">_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Histogram</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Histogram</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="clusteredColumn" uniqueId="{ECFDCEC5-6E6A-41A2-BD48-C8F84B977B67}">
@@ -606,10 +632,66 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="0"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Numbers</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Numbers</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Count</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Count</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -1171,14 +1253,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>266699</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1215,8 +1297,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6362700" y="809625"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="6362699" y="809625"/>
+              <a:ext cx="7000876" cy="3886200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1545,3014 +1627,3014 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ALL1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1000" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:1000" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
         <v>-0.29200138590608499</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>-0.22128476178965301</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>0.94240656482677099</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>-0.212825858402441</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>-0.20694918236593501</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>0.11174699938904201</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>0.298336567573734</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>3.3685331290357001E-2</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <v>0.83398843169748005</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="1">
         <v>6.5603339617612E-2</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="1">
         <v>0.28449831948951598</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="1">
         <v>-0.47847498517585602</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="1">
         <v>0.51168208531663895</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="1">
         <v>0.52073648577944798</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="1">
         <v>0.52250880366621599</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="1">
         <v>-0.53678734819206697</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="1">
         <v>0.77337165137657804</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="1">
         <v>-0.17651428693353</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="1">
         <v>-0.179895562505795</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="1">
         <v>0.47944530442463301</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="1">
         <v>-5.84557238761408E-2</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="1">
         <v>-0.32676442193322702</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="1">
         <v>-0.143892752648586</v>
       </c>
-      <c r="X1">
+      <c r="X1" s="1">
         <v>0.45431345387942901</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="1">
         <v>0.26312433999601997</v>
       </c>
-      <c r="Z1">
+      <c r="Z1" s="1">
         <v>0.72122247946408202</v>
       </c>
-      <c r="AA1">
+      <c r="AA1" s="1">
         <v>-0.70484941939536805</v>
       </c>
-      <c r="AB1">
+      <c r="AB1" s="1">
         <v>9.3870092644975298E-2</v>
       </c>
-      <c r="AC1">
+      <c r="AC1" s="1">
         <v>-0.82176861544593804</v>
       </c>
-      <c r="AD1">
+      <c r="AD1" s="1">
         <v>-0.21933519181130501</v>
       </c>
-      <c r="AE1">
+      <c r="AE1" s="1">
         <v>-0.55699156197989896</v>
       </c>
-      <c r="AF1">
+      <c r="AF1" s="1">
         <v>-0.101899770749889</v>
       </c>
-      <c r="AG1">
+      <c r="AG1" s="1">
         <v>7.9799493747441899E-2</v>
       </c>
-      <c r="AH1">
+      <c r="AH1" s="1">
         <v>-0.51416821055265305</v>
       </c>
-      <c r="AI1">
+      <c r="AI1" s="1">
         <v>0.55113873875671704</v>
       </c>
-      <c r="AJ1">
+      <c r="AJ1" s="1">
         <v>-0.17691989030084701</v>
       </c>
-      <c r="AK1">
+      <c r="AK1" s="1">
         <v>0.88495056029822705</v>
       </c>
-      <c r="AL1">
+      <c r="AL1" s="1">
         <v>-0.79965209759494005</v>
       </c>
-      <c r="AM1">
+      <c r="AM1" s="1">
         <v>-0.27284903447083098</v>
       </c>
-      <c r="AN1">
+      <c r="AN1" s="1">
         <v>-0.63432803432773899</v>
       </c>
-      <c r="AO1">
+      <c r="AO1" s="1">
         <v>-3.76796172725853E-2</v>
       </c>
-      <c r="AP1">
+      <c r="AP1" s="1">
         <v>0.233205083247911</v>
       </c>
-      <c r="AQ1">
+      <c r="AQ1" s="1">
         <v>-0.67174427192449304</v>
       </c>
-      <c r="AR1">
+      <c r="AR1" s="1">
         <v>-0.31529677682574703</v>
       </c>
-      <c r="AS1">
+      <c r="AS1" s="1">
         <v>0.58562200610367998</v>
       </c>
-      <c r="AT1">
+      <c r="AT1" s="1">
         <v>0.37982215892319698</v>
       </c>
-      <c r="AU1">
+      <c r="AU1" s="1">
         <v>-0.36194057443828997</v>
       </c>
-      <c r="AV1">
+      <c r="AV1" s="1">
         <v>-0.66951836922086005</v>
       </c>
-      <c r="AW1">
+      <c r="AW1" s="1">
         <v>0.23097893212704099</v>
       </c>
-      <c r="AX1">
+      <c r="AX1" s="1">
         <v>-0.48772709689653998</v>
       </c>
-      <c r="AY1">
+      <c r="AY1" s="1">
         <v>-0.50611682800876501</v>
       </c>
-      <c r="AZ1">
+      <c r="AZ1" s="1">
         <v>-0.24406456623876599</v>
       </c>
-      <c r="BA1">
+      <c r="BA1" s="1">
         <v>-1.4936215191368601E-2</v>
       </c>
-      <c r="BB1">
+      <c r="BB1" s="1">
         <v>7.2471432379144302E-2</v>
       </c>
-      <c r="BC1">
+      <c r="BC1" s="1">
         <v>-0.220735939913523</v>
       </c>
-      <c r="BD1">
+      <c r="BD1" s="1">
         <v>-0.42829923064352898</v>
       </c>
-      <c r="BE1">
+      <c r="BE1" s="1">
         <v>0.40405949857055601</v>
       </c>
-      <c r="BF1">
+      <c r="BF1" s="1">
         <v>5.7327388266572202E-2</v>
       </c>
-      <c r="BG1">
+      <c r="BG1" s="1">
         <v>-0.45162765123577298</v>
       </c>
-      <c r="BH1">
+      <c r="BH1" s="1">
         <v>-0.39098644142092598</v>
       </c>
-      <c r="BI1">
+      <c r="BI1" s="1">
         <v>-0.56634834674792101</v>
       </c>
-      <c r="BJ1">
+      <c r="BJ1" s="1">
         <v>0.123063639619559</v>
       </c>
-      <c r="BK1">
+      <c r="BK1" s="1">
         <v>-0.368199473094313</v>
       </c>
-      <c r="BL1">
+      <c r="BL1" s="1">
         <v>-1.07193032503728</v>
       </c>
-      <c r="BM1">
+      <c r="BM1" s="1">
         <v>-4.2587081381291997E-2</v>
       </c>
-      <c r="BN1">
+      <c r="BN1" s="1">
         <v>-0.726897604536899</v>
       </c>
-      <c r="BO1">
+      <c r="BO1" s="1">
         <v>0.18664798364504001</v>
       </c>
-      <c r="BP1">
+      <c r="BP1" s="1">
         <v>0.49163176052169599</v>
       </c>
-      <c r="BQ1">
+      <c r="BQ1" s="1">
         <v>0.67542530862454597</v>
       </c>
-      <c r="BR1">
+      <c r="BR1" s="1">
         <v>0.90102838385452799</v>
       </c>
-      <c r="BS1">
+      <c r="BS1" s="1">
         <v>-5.7677123915505502E-2</v>
       </c>
-      <c r="BT1">
+      <c r="BT1" s="1">
         <v>3.9362206649097798E-3</v>
       </c>
-      <c r="BU1">
+      <c r="BU1" s="1">
         <v>0.99923467409690003</v>
       </c>
-      <c r="BV1">
+      <c r="BV1" s="1">
         <v>0.19484187800296801</v>
       </c>
-      <c r="BW1">
+      <c r="BW1" s="1">
         <v>-0.39451985964307901</v>
       </c>
-      <c r="BX1">
+      <c r="BX1" s="1">
         <v>-0.35420909243885002</v>
       </c>
-      <c r="BY1">
+      <c r="BY1" s="1">
         <v>-0.11740176907814701</v>
       </c>
-      <c r="BZ1">
+      <c r="BZ1" s="1">
         <v>-2.6800347609502301E-2</v>
       </c>
-      <c r="CA1">
+      <c r="CA1" s="1">
         <v>0.26789840016157801</v>
       </c>
-      <c r="CB1">
+      <c r="CB1" s="1">
         <v>-0.150719321911753</v>
       </c>
-      <c r="CC1">
+      <c r="CC1" s="1">
         <v>-0.15302459693305001</v>
       </c>
-      <c r="CD1">
+      <c r="CD1" s="1">
         <v>6.0755169528618702E-2</v>
       </c>
-      <c r="CE1">
+      <c r="CE1" s="1">
         <v>0.209436182983335</v>
       </c>
-      <c r="CF1">
+      <c r="CF1" s="1">
         <v>-0.20090622249044199</v>
       </c>
-      <c r="CG1">
+      <c r="CG1" s="1">
         <v>-0.36006650525727601</v>
       </c>
-      <c r="CH1">
+      <c r="CH1" s="1">
         <v>0.78951517540048399</v>
       </c>
-      <c r="CI1">
+      <c r="CI1" s="1">
         <v>0.94772943599407899</v>
       </c>
-      <c r="CJ1">
+      <c r="CJ1" s="1">
         <v>0.28703790821209901</v>
       </c>
-      <c r="CK1">
+      <c r="CK1" s="1">
         <v>-6.4524933046921903E-2</v>
       </c>
-      <c r="CL1">
+      <c r="CL1" s="1">
         <v>-0.26448660494495901</v>
       </c>
-      <c r="CM1">
+      <c r="CM1" s="1">
         <v>0.34043184140510402</v>
       </c>
-      <c r="CN1">
+      <c r="CN1" s="1">
         <v>0.37989582550818501</v>
       </c>
-      <c r="CO1">
+      <c r="CO1" s="1">
         <v>0.40693004285226497</v>
       </c>
-      <c r="CP1">
+      <c r="CP1" s="1">
         <v>-0.35413070493377802</v>
       </c>
-      <c r="CQ1">
+      <c r="CQ1" s="1">
         <v>0.69682846617231597</v>
       </c>
-      <c r="CR1">
+      <c r="CR1" s="1">
         <v>0.84056582732470497</v>
       </c>
-      <c r="CS1">
+      <c r="CS1" s="1">
         <v>-1.0781257493245899</v>
       </c>
-      <c r="CT1">
+      <c r="CT1" s="1">
         <v>-0.24336383525712799</v>
       </c>
-      <c r="CU1">
+      <c r="CU1" s="1">
         <v>-0.53807507621540696</v>
       </c>
-      <c r="CV1">
+      <c r="CV1" s="1">
         <v>0.15902335196057901</v>
       </c>
-      <c r="CW1">
+      <c r="CW1" s="1">
         <v>-0.69062860144480998</v>
       </c>
-      <c r="CX1">
+      <c r="CX1" s="1">
         <v>-0.51681988003664303</v>
       </c>
-      <c r="CY1">
+      <c r="CY1" s="1">
         <v>0.24485399549822101</v>
       </c>
-      <c r="CZ1">
+      <c r="CZ1" s="1">
         <v>-0.25349141889420501</v>
       </c>
-      <c r="DA1">
+      <c r="DA1" s="1">
         <v>0.55324088077461997</v>
       </c>
-      <c r="DB1">
+      <c r="DB1" s="1">
         <v>9.2029740208497995E-2</v>
       </c>
-      <c r="DC1">
+      <c r="DC1" s="1">
         <v>0.26250323813722098</v>
       </c>
-      <c r="DD1">
+      <c r="DD1" s="1">
         <v>0.29997824436223802</v>
       </c>
-      <c r="DE1">
+      <c r="DE1" s="1">
         <v>-0.26369278777379501</v>
       </c>
-      <c r="DF1">
+      <c r="DF1" s="1">
         <v>-0.48041733879242099</v>
       </c>
-      <c r="DG1">
+      <c r="DG1" s="1">
         <v>7.8880030448571697E-2</v>
       </c>
-      <c r="DH1">
+      <c r="DH1" s="1">
         <v>-0.31369717047086598</v>
       </c>
-      <c r="DI1">
+      <c r="DI1" s="1">
         <v>-0.18114241714516499</v>
       </c>
-      <c r="DJ1">
+      <c r="DJ1" s="1">
         <v>-0.34667359952068499</v>
       </c>
-      <c r="DK1">
+      <c r="DK1" s="1">
         <v>-0.12828613641211101</v>
       </c>
-      <c r="DL1">
+      <c r="DL1" s="1">
         <v>-0.11866074783130399</v>
       </c>
-      <c r="DM1">
+      <c r="DM1" s="1">
         <v>-2.7790348822401102E-2</v>
       </c>
-      <c r="DN1">
+      <c r="DN1" s="1">
         <v>-0.79001478024719995</v>
       </c>
-      <c r="DO1">
+      <c r="DO1" s="1">
         <v>-0.111604476556525</v>
       </c>
-      <c r="DP1">
+      <c r="DP1" s="1">
         <v>-0.461221647645426</v>
       </c>
-      <c r="DQ1">
+      <c r="DQ1" s="1">
         <v>-0.21466157913543699</v>
       </c>
-      <c r="DR1">
+      <c r="DR1" s="1">
         <v>-0.39018385184354198</v>
       </c>
-      <c r="DS1">
+      <c r="DS1" s="1">
         <v>-0.17916682908815201</v>
       </c>
-      <c r="DT1">
+      <c r="DT1" s="1">
         <v>-0.70581390791394105</v>
       </c>
-      <c r="DU1">
+      <c r="DU1" s="1">
         <v>0.36227994173704597</v>
       </c>
-      <c r="DV1">
+      <c r="DV1" s="1">
         <v>0.272104484020184</v>
       </c>
-      <c r="DW1">
+      <c r="DW1" s="1">
         <v>0.22339115387926001</v>
       </c>
-      <c r="DX1">
+      <c r="DX1" s="1">
         <v>0.19203857565507201</v>
       </c>
-      <c r="DY1">
+      <c r="DY1" s="1">
         <v>0.68200212562745499</v>
       </c>
-      <c r="DZ1">
+      <c r="DZ1" s="1">
         <v>0.206002654293614</v>
       </c>
-      <c r="EA1">
+      <c r="EA1" s="1">
         <v>-0.29903047456885501</v>
       </c>
-      <c r="EB1">
+      <c r="EB1" s="1">
         <v>0.35800919190774699</v>
       </c>
-      <c r="EC1">
+      <c r="EC1" s="1">
         <v>-0.30846757032114602</v>
       </c>
-      <c r="ED1">
+      <c r="ED1" s="1">
         <v>-0.48948228870271199</v>
       </c>
-      <c r="EE1">
+      <c r="EE1" s="1">
         <v>-8.8122114901663606E-2</v>
       </c>
-      <c r="EF1">
+      <c r="EF1" s="1">
         <v>0.70569171361148297</v>
       </c>
-      <c r="EG1">
+      <c r="EG1" s="1">
         <v>-0.48879513913343697</v>
       </c>
-      <c r="EH1">
+      <c r="EH1" s="1">
         <v>0.52698258718488</v>
       </c>
-      <c r="EI1">
+      <c r="EI1" s="1">
         <v>0.310560672680677</v>
       </c>
-      <c r="EJ1">
+      <c r="EJ1" s="1">
         <v>-1.5648941821509301E-2</v>
       </c>
-      <c r="EK1">
+      <c r="EK1" s="1">
         <v>-5.8297125345643998E-2</v>
       </c>
-      <c r="EL1">
+      <c r="EL1" s="1">
         <v>-0.67575270284037803</v>
       </c>
-      <c r="EM1">
+      <c r="EM1" s="1">
         <v>-3.3867169264767599E-2</v>
       </c>
-      <c r="EN1">
+      <c r="EN1" s="1">
         <v>-0.46906683489006501</v>
       </c>
-      <c r="EO1">
+      <c r="EO1" s="1">
         <v>-0.33959956870494501</v>
       </c>
-      <c r="EP1">
+      <c r="EP1" s="1">
         <v>0.16983914976347</v>
       </c>
-      <c r="EQ1">
+      <c r="EQ1" s="1">
         <v>0.30706271056566398</v>
       </c>
-      <c r="ER1">
+      <c r="ER1" s="1">
         <v>-0.49801535147181802</v>
       </c>
-      <c r="ES1">
+      <c r="ES1" s="1">
         <v>-0.21350606449237999</v>
       </c>
-      <c r="ET1">
+      <c r="ET1" s="1">
         <v>7.9732596040909196E-2</v>
       </c>
-      <c r="EU1">
+      <c r="EU1" s="1">
         <v>-0.53133892739362898</v>
       </c>
-      <c r="EV1">
+      <c r="EV1" s="1">
         <v>9.5473773752088195E-2</v>
       </c>
-      <c r="EW1">
+      <c r="EW1" s="1">
         <v>-0.282996867953829</v>
       </c>
-      <c r="EX1">
+      <c r="EX1" s="1">
         <v>0.51092102675678097</v>
       </c>
-      <c r="EY1">
+      <c r="EY1" s="1">
         <v>-0.499529826236355</v>
       </c>
-      <c r="EZ1">
+      <c r="EZ1" s="1">
         <v>0.476002438642184</v>
       </c>
-      <c r="FA1">
+      <c r="FA1" s="1">
         <v>0.51166413401397004</v>
       </c>
-      <c r="FB1">
+      <c r="FB1" s="1">
         <v>-0.43984772327278399</v>
       </c>
-      <c r="FC1">
+      <c r="FC1" s="1">
         <v>-0.39003451382927001</v>
       </c>
-      <c r="FD1">
+      <c r="FD1" s="1">
         <v>-0.36644336786551601</v>
       </c>
-      <c r="FE1">
+      <c r="FE1" s="1">
         <v>1.09881847304989</v>
       </c>
-      <c r="FF1">
+      <c r="FF1" s="1">
         <v>2.3152760115433501E-2</v>
       </c>
-      <c r="FG1">
+      <c r="FG1" s="1">
         <v>0.18104925025382701</v>
       </c>
-      <c r="FH1">
+      <c r="FH1" s="1">
         <v>-0.16918761594975801</v>
       </c>
-      <c r="FI1">
+      <c r="FI1" s="1">
         <v>0.65989545946440997</v>
       </c>
-      <c r="FJ1">
+      <c r="FJ1" s="1">
         <v>0.38198749477014499</v>
       </c>
-      <c r="FK1">
+      <c r="FK1" s="1">
         <v>-0.42667146533481598</v>
       </c>
-      <c r="FL1">
+      <c r="FL1" s="1">
         <v>0.46584516215789901</v>
       </c>
-      <c r="FM1">
+      <c r="FM1" s="1">
         <v>0.14078121758806</v>
       </c>
-      <c r="FN1">
+      <c r="FN1" s="1">
         <v>-0.306913278122455</v>
       </c>
-      <c r="FO1">
+      <c r="FO1" s="1">
         <v>0.18348153605204801</v>
       </c>
-      <c r="FP1">
+      <c r="FP1" s="1">
         <v>2.92647201888942E-2</v>
       </c>
-      <c r="FQ1">
+      <c r="FQ1" s="1">
         <v>0.15264543733570901</v>
       </c>
-      <c r="FR1">
+      <c r="FR1" s="1">
         <v>-1.04134679654171</v>
       </c>
-      <c r="FS1">
+      <c r="FS1" s="1">
         <v>-0.35710375050056897</v>
       </c>
-      <c r="FT1">
+      <c r="FT1" s="1">
         <v>-4.9189388937640403E-2</v>
       </c>
-      <c r="FU1">
+      <c r="FU1" s="1">
         <v>-1.4952252887191599</v>
       </c>
-      <c r="FV1">
+      <c r="FV1" s="1">
         <v>-0.72251850261705997</v>
       </c>
-      <c r="FW1">
+      <c r="FW1" s="1">
         <v>-0.167542485096736</v>
       </c>
-      <c r="FX1">
+      <c r="FX1" s="1">
         <v>-0.77422421743560998</v>
       </c>
-      <c r="FY1">
+      <c r="FY1" s="1">
         <v>0.61136302069000503</v>
       </c>
-      <c r="FZ1">
+      <c r="FZ1" s="1">
         <v>-0.83174791224459599</v>
       </c>
-      <c r="GA1">
+      <c r="GA1" s="1">
         <v>-0.48911139924703601</v>
       </c>
-      <c r="GB1">
+      <c r="GB1" s="1">
         <v>-0.43588978833166397</v>
       </c>
-      <c r="GC1">
+      <c r="GC1" s="1">
         <v>-0.24094386451359501</v>
       </c>
-      <c r="GD1">
+      <c r="GD1" s="1">
         <v>0.54906562047146801</v>
       </c>
-      <c r="GE1">
+      <c r="GE1" s="1">
         <v>-0.71455328756648695</v>
       </c>
-      <c r="GF1">
+      <c r="GF1" s="1">
         <v>-1.2346693658043999</v>
       </c>
-      <c r="GG1">
+      <c r="GG1" s="1">
         <v>0.94974151739225898</v>
       </c>
-      <c r="GH1">
+      <c r="GH1" s="1">
         <v>1.0236261932281501</v>
       </c>
-      <c r="GI1">
+      <c r="GI1" s="1">
         <v>0.53455858369310705</v>
       </c>
-      <c r="GJ1">
+      <c r="GJ1" s="1">
         <v>-0.238576239316908</v>
       </c>
-      <c r="GK1">
+      <c r="GK1" s="1">
         <v>-0.85722611275342997</v>
       </c>
-      <c r="GL1">
+      <c r="GL1" s="1">
         <v>0.35125073014270503</v>
       </c>
-      <c r="GM1">
+      <c r="GM1" s="1">
         <v>-9.3055864945351105E-2</v>
       </c>
-      <c r="GN1">
+      <c r="GN1" s="1">
         <v>-7.9241628467515798E-2</v>
       </c>
-      <c r="GO1">
+      <c r="GO1" s="1">
         <v>0.21455078716767001</v>
       </c>
-      <c r="GP1">
+      <c r="GP1" s="1">
         <v>0.224625309176153</v>
       </c>
-      <c r="GQ1">
+      <c r="GQ1" s="1">
         <v>-0.45261552142720501</v>
       </c>
-      <c r="GR1">
+      <c r="GR1" s="1">
         <v>-0.18278305958254601</v>
       </c>
-      <c r="GS1">
+      <c r="GS1" s="1">
         <v>0.84868058009167102</v>
       </c>
-      <c r="GT1">
+      <c r="GT1" s="1">
         <v>-0.49804004573558602</v>
       </c>
-      <c r="GU1">
+      <c r="GU1" s="1">
         <v>-0.33477488210240097</v>
       </c>
-      <c r="GV1">
+      <c r="GV1" s="1">
         <v>0.35262699743394599</v>
       </c>
-      <c r="GW1">
+      <c r="GW1" s="1">
         <v>-0.13912058532015201</v>
       </c>
-      <c r="GX1">
+      <c r="GX1" s="1">
         <v>-4.2375148609789699E-2</v>
       </c>
-      <c r="GY1">
+      <c r="GY1" s="1">
         <v>0.54015050613994697</v>
       </c>
-      <c r="GZ1">
+      <c r="GZ1" s="1">
         <v>0.44747996491566799</v>
       </c>
-      <c r="HA1">
+      <c r="HA1" s="1">
         <v>-0.76710515141639102</v>
       </c>
-      <c r="HB1">
+      <c r="HB1" s="1">
         <v>-0.60349957521685604</v>
       </c>
-      <c r="HC1">
+      <c r="HC1" s="1">
         <v>-0.151184199474963</v>
       </c>
-      <c r="HD1">
+      <c r="HD1" s="1">
         <v>0.492993188187904</v>
       </c>
-      <c r="HE1">
+      <c r="HE1" s="1">
         <v>1.0870006833139001</v>
       </c>
-      <c r="HF1">
+      <c r="HF1" s="1">
         <v>-0.36538219668583199</v>
       </c>
-      <c r="HG1">
+      <c r="HG1" s="1">
         <v>-2.8813456851274399E-2</v>
       </c>
-      <c r="HH1">
+      <c r="HH1" s="1">
         <v>-1.37623714864951</v>
       </c>
-      <c r="HI1">
+      <c r="HI1" s="1">
         <v>0.75498668857855</v>
       </c>
-      <c r="HJ1">
+      <c r="HJ1" s="1">
         <v>-0.243706058037541</v>
       </c>
-      <c r="HK1">
+      <c r="HK1" s="1">
         <v>-0.176628204015952</v>
       </c>
-      <c r="HL1">
+      <c r="HL1" s="1">
         <v>0.33508984944745601</v>
       </c>
-      <c r="HM1">
+      <c r="HM1" s="1">
         <v>0.221581980228751</v>
       </c>
-      <c r="HN1">
+      <c r="HN1" s="1">
         <v>0.59705782278712205</v>
       </c>
-      <c r="HO1">
+      <c r="HO1" s="1">
         <v>9.6645451047774403E-2</v>
       </c>
-      <c r="HP1">
+      <c r="HP1" s="1">
         <v>0.46380440833291903</v>
       </c>
-      <c r="HQ1">
+      <c r="HQ1" s="1">
         <v>-0.39087297834598</v>
       </c>
-      <c r="HR1">
+      <c r="HR1" s="1">
         <v>-0.66787086098423198</v>
       </c>
-      <c r="HS1">
+      <c r="HS1" s="1">
         <v>-0.197747411704322</v>
       </c>
-      <c r="HT1">
+      <c r="HT1" s="1">
         <v>0.72641426209626203</v>
       </c>
-      <c r="HU1">
+      <c r="HU1" s="1">
         <v>-8.6210990310289295E-2</v>
       </c>
-      <c r="HV1">
+      <c r="HV1" s="1">
         <v>0.127524310046185</v>
       </c>
-      <c r="HW1">
+      <c r="HW1" s="1">
         <v>6.1739592850570103E-2</v>
       </c>
-      <c r="HX1">
+      <c r="HX1" s="1">
         <v>0.23515227075093401</v>
       </c>
-      <c r="HY1">
+      <c r="HY1" s="1">
         <v>0.42808109621255602</v>
       </c>
-      <c r="HZ1">
+      <c r="HZ1" s="1">
         <v>0.84814884948716895</v>
       </c>
-      <c r="IA1">
+      <c r="IA1" s="1">
         <v>-0.28714166275300201</v>
       </c>
-      <c r="IB1">
+      <c r="IB1" s="1">
         <v>0.62030612628528703</v>
       </c>
-      <c r="IC1">
+      <c r="IC1" s="1">
         <v>0.80269799413718801</v>
       </c>
-      <c r="ID1">
+      <c r="ID1" s="1">
         <v>-1.3679144458472201</v>
       </c>
-      <c r="IE1">
+      <c r="IE1" s="1">
         <v>-0.60540905239181997</v>
       </c>
-      <c r="IF1">
+      <c r="IF1" s="1">
         <v>-0.730809323247544</v>
       </c>
-      <c r="IG1">
+      <c r="IG1" s="1">
         <v>0.61647176380183899</v>
       </c>
-      <c r="IH1">
+      <c r="IH1" s="1">
         <v>-0.10471555581153499</v>
       </c>
-      <c r="II1">
+      <c r="II1" s="1">
         <v>-0.390347529887282</v>
       </c>
-      <c r="IJ1">
+      <c r="IJ1" s="1">
         <v>-0.30673442612778001</v>
       </c>
-      <c r="IK1">
+      <c r="IK1" s="1">
         <v>0.37896961665173601</v>
       </c>
-      <c r="IL1">
+      <c r="IL1" s="1">
         <v>-1.01926305897226</v>
       </c>
-      <c r="IM1">
+      <c r="IM1" s="1">
         <v>-0.49417806596883601</v>
       </c>
-      <c r="IN1">
+      <c r="IN1" s="1">
         <v>0.60953093889143695</v>
       </c>
-      <c r="IO1">
+      <c r="IO1" s="1">
         <v>0.28189927132117998</v>
       </c>
-      <c r="IP1">
+      <c r="IP1" s="1">
         <v>-0.72517209299384899</v>
       </c>
-      <c r="IQ1">
+      <c r="IQ1" s="1">
         <v>-0.37928091426399102</v>
       </c>
-      <c r="IR1">
+      <c r="IR1" s="1">
         <v>-0.149133941363186</v>
       </c>
-      <c r="IS1">
+      <c r="IS1" s="1">
         <v>-0.36975495975294698</v>
       </c>
-      <c r="IT1">
+      <c r="IT1" s="1">
         <v>-0.266223623109614</v>
       </c>
-      <c r="IU1">
+      <c r="IU1" s="1">
         <v>-0.13540499243822901</v>
       </c>
-      <c r="IV1">
+      <c r="IV1" s="1">
         <v>-0.15327339293998599</v>
       </c>
-      <c r="IW1">
+      <c r="IW1" s="1">
         <v>7.8901668292843494E-2</v>
       </c>
-      <c r="IX1">
+      <c r="IX1" s="1">
         <v>-4.3708624223658303E-3</v>
       </c>
-      <c r="IY1">
+      <c r="IY1" s="1">
         <v>-0.80971337183139802</v>
       </c>
-      <c r="IZ1">
+      <c r="IZ1" s="1">
         <v>0.262500382445914</v>
       </c>
-      <c r="JA1">
+      <c r="JA1" s="1">
         <v>-0.60456514001284101</v>
       </c>
-      <c r="JB1">
+      <c r="JB1" s="1">
         <v>-3.7524562669011399E-2</v>
       </c>
-      <c r="JC1">
+      <c r="JC1" s="1">
         <v>-0.98045987336551799</v>
       </c>
-      <c r="JD1">
+      <c r="JD1" s="1">
         <v>-0.515678849989469</v>
       </c>
-      <c r="JE1">
+      <c r="JE1" s="1">
         <v>-1.07281505022976E-2</v>
       </c>
-      <c r="JF1">
+      <c r="JF1" s="1">
         <v>2.1281770257817901E-2</v>
       </c>
-      <c r="JG1">
+      <c r="JG1" s="1">
         <v>-0.24416421531361801</v>
       </c>
-      <c r="JH1">
+      <c r="JH1" s="1">
         <v>0.12712123397854599</v>
       </c>
-      <c r="JI1">
+      <c r="JI1" s="1">
         <v>0.26764836343210402</v>
       </c>
-      <c r="JJ1">
+      <c r="JJ1" s="1">
         <v>-0.14003005949879899</v>
       </c>
-      <c r="JK1">
+      <c r="JK1" s="1">
         <v>0.36331545504642498</v>
       </c>
-      <c r="JL1">
+      <c r="JL1" s="1">
         <v>-0.24819436838838699</v>
       </c>
-      <c r="JM1">
+      <c r="JM1" s="1">
         <v>0.15383114312311999</v>
       </c>
-      <c r="JN1">
+      <c r="JN1" s="1">
         <v>-0.30815173425458298</v>
       </c>
-      <c r="JO1">
+      <c r="JO1" s="1">
         <v>9.0369414810857501E-2</v>
       </c>
-      <c r="JP1">
+      <c r="JP1" s="1">
         <v>-0.18586866595180099</v>
       </c>
-      <c r="JQ1">
+      <c r="JQ1" s="1">
         <v>-1.40345505134382</v>
       </c>
-      <c r="JR1">
+      <c r="JR1" s="1">
         <v>0.41731294822265602</v>
       </c>
-      <c r="JS1">
+      <c r="JS1" s="1">
         <v>-0.73628896360706197</v>
       </c>
-      <c r="JT1">
+      <c r="JT1" s="1">
         <v>-0.47698913720585001</v>
       </c>
-      <c r="JU1">
+      <c r="JU1" s="1">
         <v>0.30899068259232898</v>
       </c>
-      <c r="JV1">
+      <c r="JV1" s="1">
         <v>-0.22397679782016</v>
       </c>
-      <c r="JW1">
+      <c r="JW1" s="1">
         <v>1.32230154217121E-2</v>
       </c>
-      <c r="JX1">
+      <c r="JX1" s="1">
         <v>-0.48689599790086502</v>
       </c>
-      <c r="JY1">
+      <c r="JY1" s="1">
         <v>0.69484149496833203</v>
       </c>
-      <c r="JZ1">
+      <c r="JZ1" s="1">
         <v>-0.81985777130914095</v>
       </c>
-      <c r="KA1">
+      <c r="KA1" s="1">
         <v>-3.6858328012682101E-2</v>
       </c>
-      <c r="KB1">
+      <c r="KB1" s="1">
         <v>0.47337451935173303</v>
       </c>
-      <c r="KC1">
+      <c r="KC1" s="1">
         <v>-0.12625480247420301</v>
       </c>
-      <c r="KD1">
+      <c r="KD1" s="1">
         <v>-7.1517212074169001E-2</v>
       </c>
-      <c r="KE1">
+      <c r="KE1" s="1">
         <v>-0.92854727076201404</v>
       </c>
-      <c r="KF1">
+      <c r="KF1" s="1">
         <v>-2.7561732531891401E-2</v>
       </c>
-      <c r="KG1">
+      <c r="KG1" s="1">
         <v>9.5579886685384904E-2</v>
       </c>
-      <c r="KH1">
+      <c r="KH1" s="1">
         <v>2.1188662468943999E-2</v>
       </c>
-      <c r="KI1">
+      <c r="KI1" s="1">
         <v>-0.72429192486231198</v>
       </c>
-      <c r="KJ1">
+      <c r="KJ1" s="1">
         <v>0.36082892364943098</v>
       </c>
-      <c r="KK1">
+      <c r="KK1" s="1">
         <v>0.48812199573201098</v>
       </c>
-      <c r="KL1">
+      <c r="KL1" s="1">
         <v>-0.30290209385996197</v>
       </c>
-      <c r="KM1">
+      <c r="KM1" s="1">
         <v>-0.185890827586428</v>
       </c>
-      <c r="KN1">
+      <c r="KN1" s="1">
         <v>-0.214453682976434</v>
       </c>
-      <c r="KO1">
+      <c r="KO1" s="1">
         <v>-7.5627088965633096E-2</v>
       </c>
-      <c r="KP1">
+      <c r="KP1" s="1">
         <v>0.40449565571139001</v>
       </c>
-      <c r="KQ1">
+      <c r="KQ1" s="1">
         <v>-6.9455990925633801E-2</v>
       </c>
-      <c r="KR1">
+      <c r="KR1" s="1">
         <v>0.47350149111001399</v>
       </c>
-      <c r="KS1">
+      <c r="KS1" s="1">
         <v>0.31395803640798697</v>
       </c>
-      <c r="KT1">
+      <c r="KT1" s="1">
         <v>-0.357608782346785</v>
       </c>
-      <c r="KU1">
+      <c r="KU1" s="1">
         <v>-0.45763858722084599</v>
       </c>
-      <c r="KV1">
+      <c r="KV1" s="1">
         <v>0.170508719130779</v>
       </c>
-      <c r="KW1">
+      <c r="KW1" s="1">
         <v>3.60177936808714E-2</v>
       </c>
-      <c r="KX1">
+      <c r="KX1" s="1">
         <v>-0.20746283995082901</v>
       </c>
-      <c r="KY1">
+      <c r="KY1" s="1">
         <v>-2.1126227074552101E-2</v>
       </c>
-      <c r="KZ1">
+      <c r="KZ1" s="1">
         <v>0.15828732862570599</v>
       </c>
-      <c r="LA1">
+      <c r="LA1" s="1">
         <v>-0.50109614739630504</v>
       </c>
-      <c r="LB1">
+      <c r="LB1" s="1">
         <v>3.1751452565975002E-2</v>
       </c>
-      <c r="LC1">
+      <c r="LC1" s="1">
         <v>0.155967264749863</v>
       </c>
-      <c r="LD1">
+      <c r="LD1" s="1">
         <v>-0.170966695045074</v>
       </c>
-      <c r="LE1">
+      <c r="LE1" s="1">
         <v>0.16437562877042999</v>
       </c>
-      <c r="LF1">
+      <c r="LF1" s="1">
         <v>0.12576143062933201</v>
       </c>
-      <c r="LG1">
+      <c r="LG1" s="1">
         <v>0.40572601756730498</v>
       </c>
-      <c r="LH1">
+      <c r="LH1" s="1">
         <v>-0.162463927534856</v>
       </c>
-      <c r="LI1">
+      <c r="LI1" s="1">
         <v>-9.0481881100293302E-2</v>
       </c>
-      <c r="LJ1">
+      <c r="LJ1" s="1">
         <v>0.224872725912031</v>
       </c>
-      <c r="LK1">
+      <c r="LK1" s="1">
         <v>0.22971109459252101</v>
       </c>
-      <c r="LL1">
+      <c r="LL1" s="1">
         <v>0.24976937682203501</v>
       </c>
-      <c r="LM1">
+      <c r="LM1" s="1">
         <v>-0.44702748492149902</v>
       </c>
-      <c r="LN1">
+      <c r="LN1" s="1">
         <v>0.27413148047177199</v>
       </c>
-      <c r="LO1">
+      <c r="LO1" s="1">
         <v>0.32013780435815398</v>
       </c>
-      <c r="LP1">
+      <c r="LP1" s="1">
         <v>9.2320353649783301E-3</v>
       </c>
-      <c r="LQ1">
+      <c r="LQ1" s="1">
         <v>0.56317985411756899</v>
       </c>
-      <c r="LR1">
+      <c r="LR1" s="1">
         <v>0.57426381911929603</v>
       </c>
-      <c r="LS1">
+      <c r="LS1" s="1">
         <v>0.33957577102451197</v>
       </c>
-      <c r="LT1">
+      <c r="LT1" s="1">
         <v>5.8656346281423702E-2</v>
       </c>
-      <c r="LU1">
+      <c r="LU1" s="1">
         <v>-0.432851511701698</v>
       </c>
-      <c r="LV1">
+      <c r="LV1" s="1">
         <v>0.176323083127294</v>
       </c>
-      <c r="LW1">
+      <c r="LW1" s="1">
         <v>-7.1336111570067695E-2</v>
       </c>
-      <c r="LX1">
+      <c r="LX1" s="1">
         <v>0.17812955623795099</v>
       </c>
-      <c r="LY1">
+      <c r="LY1" s="1">
         <v>-0.41055232892056498</v>
       </c>
-      <c r="LZ1">
+      <c r="LZ1" s="1">
         <v>-0.26964301498624299</v>
       </c>
-      <c r="MA1">
+      <c r="MA1" s="1">
         <v>1.5081213992615E-2</v>
       </c>
-      <c r="MB1">
+      <c r="MB1" s="1">
         <v>-0.90802794701210998</v>
       </c>
-      <c r="MC1">
+      <c r="MC1" s="1">
         <v>-6.27284079140369E-3</v>
       </c>
-      <c r="MD1">
+      <c r="MD1" s="1">
         <v>-0.31721750010307498</v>
       </c>
-      <c r="ME1">
+      <c r="ME1" s="1">
         <v>-0.88335193776697896</v>
       </c>
-      <c r="MF1">
+      <c r="MF1" s="1">
         <v>1.6099308988651698E-2</v>
       </c>
-      <c r="MG1">
+      <c r="MG1" s="1">
         <v>1.30319086918171</v>
       </c>
-      <c r="MH1">
+      <c r="MH1" s="1">
         <v>7.0205075724591406E-2</v>
       </c>
-      <c r="MI1">
+      <c r="MI1" s="1">
         <v>0.58064130762697197</v>
       </c>
-      <c r="MJ1">
+      <c r="MJ1" s="1">
         <v>0.34028577386749698</v>
       </c>
-      <c r="MK1">
+      <c r="MK1" s="1">
         <v>-0.412192052545234</v>
       </c>
-      <c r="ML1">
+      <c r="ML1" s="1">
         <v>-0.80241468890676504</v>
       </c>
-      <c r="MM1">
+      <c r="MM1" s="1">
         <v>2.4279077289153701E-2</v>
       </c>
-      <c r="MN1">
+      <c r="MN1" s="1">
         <v>2.90820328518437E-2</v>
       </c>
-      <c r="MO1">
+      <c r="MO1" s="1">
         <v>-0.86377566068834</v>
       </c>
-      <c r="MP1">
+      <c r="MP1" s="1">
         <v>-0.32245010669311702</v>
       </c>
-      <c r="MQ1">
+      <c r="MQ1" s="1">
         <v>0.25210967832999398</v>
       </c>
-      <c r="MR1">
+      <c r="MR1" s="1">
         <v>-0.74200935628331399</v>
       </c>
-      <c r="MS1">
+      <c r="MS1" s="1">
         <v>0.35478252661800802</v>
       </c>
-      <c r="MT1">
+      <c r="MT1" s="1">
         <v>-0.58269011421954497</v>
       </c>
-      <c r="MU1">
+      <c r="MU1" s="1">
         <v>-0.13640888828054601</v>
       </c>
-      <c r="MV1">
+      <c r="MV1" s="1">
         <v>-3.54765815770458E-2</v>
       </c>
-      <c r="MW1">
+      <c r="MW1" s="1">
         <v>0.248639651465624</v>
       </c>
-      <c r="MX1">
+      <c r="MX1" s="1">
         <v>-0.32307499048076599</v>
       </c>
-      <c r="MY1">
+      <c r="MY1" s="1">
         <v>0.38508872070160299</v>
       </c>
-      <c r="MZ1">
+      <c r="MZ1" s="1">
         <v>1.5466957823404799E-2</v>
       </c>
-      <c r="NA1">
+      <c r="NA1" s="1">
         <v>-0.91718302428699805</v>
       </c>
-      <c r="NB1">
+      <c r="NB1" s="1">
         <v>-0.36334267186659502</v>
       </c>
-      <c r="NC1">
+      <c r="NC1" s="1">
         <v>6.0094033467713798E-3</v>
       </c>
-      <c r="ND1">
+      <c r="ND1" s="1">
         <v>-0.54436033735664802</v>
       </c>
-      <c r="NE1">
+      <c r="NE1" s="1">
         <v>-1.05668054834848</v>
       </c>
-      <c r="NF1">
+      <c r="NF1" s="1">
         <v>-0.77483653316349999</v>
       </c>
-      <c r="NG1">
+      <c r="NG1" s="1">
         <v>-0.75791537292738498</v>
       </c>
-      <c r="NH1">
+      <c r="NH1" s="1">
         <v>0.80374191924857297</v>
       </c>
-      <c r="NI1">
+      <c r="NI1" s="1">
         <v>-0.44059113724716997</v>
       </c>
-      <c r="NJ1">
+      <c r="NJ1" s="1">
         <v>-7.3467231901242103E-2</v>
       </c>
-      <c r="NK1">
+      <c r="NK1" s="1">
         <v>0.706443532094295</v>
       </c>
-      <c r="NL1">
+      <c r="NL1" s="1">
         <v>-6.0669023489966702E-2</v>
       </c>
-      <c r="NM1">
+      <c r="NM1" s="1">
         <v>-5.0462731925988102E-2</v>
       </c>
-      <c r="NN1">
+      <c r="NN1" s="1">
         <v>0.65230344772255999</v>
       </c>
-      <c r="NO1">
+      <c r="NO1" s="1">
         <v>0.21972098750743399</v>
       </c>
-      <c r="NP1">
+      <c r="NP1" s="1">
         <v>-0.34797763085470901</v>
       </c>
-      <c r="NQ1">
+      <c r="NQ1" s="1">
         <v>-0.35393391314204597</v>
       </c>
-      <c r="NR1">
+      <c r="NR1" s="1">
         <v>-0.19391547909221199</v>
       </c>
-      <c r="NS1">
+      <c r="NS1" s="1">
         <v>0.261878106225575</v>
       </c>
-      <c r="NT1">
+      <c r="NT1" s="1">
         <v>-0.174203728093764</v>
       </c>
-      <c r="NU1">
+      <c r="NU1" s="1">
         <v>0.408601764710606</v>
       </c>
-      <c r="NV1">
+      <c r="NV1" s="1">
         <v>-0.53287764525994596</v>
       </c>
-      <c r="NW1">
+      <c r="NW1" s="1">
         <v>0.71713008439454695</v>
       </c>
-      <c r="NX1">
+      <c r="NX1" s="1">
         <v>0.31930451332100301</v>
       </c>
-      <c r="NY1">
+      <c r="NY1" s="1">
         <v>0.17551385942235501</v>
       </c>
-      <c r="NZ1">
+      <c r="NZ1" s="1">
         <v>0.29097745156986299</v>
       </c>
-      <c r="OA1">
+      <c r="OA1" s="1">
         <v>0.209345379704863</v>
       </c>
-      <c r="OB1">
+      <c r="OB1" s="1">
         <v>-1.82189121268278E-3</v>
       </c>
-      <c r="OC1">
+      <c r="OC1" s="1">
         <v>0.54500202363408601</v>
       </c>
-      <c r="OD1">
+      <c r="OD1" s="1">
         <v>0.60173133478600604</v>
       </c>
-      <c r="OE1">
+      <c r="OE1" s="1">
         <v>-0.36398872442387997</v>
       </c>
-      <c r="OF1">
+      <c r="OF1" s="1">
         <v>1.0744033909095501</v>
       </c>
-      <c r="OG1">
+      <c r="OG1" s="1">
         <v>0.119146042290183</v>
       </c>
-      <c r="OH1">
+      <c r="OH1" s="1">
         <v>0.96591907106345698</v>
       </c>
-      <c r="OI1">
+      <c r="OI1" s="1">
         <v>-0.22591626486599301</v>
       </c>
-      <c r="OJ1">
+      <c r="OJ1" s="1">
         <v>-0.45725869479625503</v>
       </c>
-      <c r="OK1">
+      <c r="OK1" s="1">
         <v>-1.14019759162115</v>
       </c>
-      <c r="OL1">
+      <c r="OL1" s="1">
         <v>0.811200638110676</v>
       </c>
-      <c r="OM1">
+      <c r="OM1" s="1">
         <v>5.8467076284444301E-2</v>
       </c>
-      <c r="ON1">
+      <c r="ON1" s="1">
         <v>0.61860235220951598</v>
       </c>
-      <c r="OO1">
+      <c r="OO1" s="1">
         <v>8.7807297242522807E-3</v>
       </c>
-      <c r="OP1">
+      <c r="OP1" s="1">
         <v>0.51730138509187695</v>
       </c>
-      <c r="OQ1">
+      <c r="OQ1" s="1">
         <v>-0.81484177189572304</v>
       </c>
-      <c r="OR1">
+      <c r="OR1" s="1">
         <v>-0.12219578761748801</v>
       </c>
-      <c r="OS1">
+      <c r="OS1" s="1">
         <v>-0.57997418646199606</v>
       </c>
-      <c r="OT1">
+      <c r="OT1" s="1">
         <v>0.49495070648599898</v>
       </c>
-      <c r="OU1">
+      <c r="OU1" s="1">
         <v>0.10456768877240601</v>
       </c>
-      <c r="OV1">
+      <c r="OV1" s="1">
         <v>-0.81118300732529303</v>
       </c>
-      <c r="OW1">
+      <c r="OW1" s="1">
         <v>0.43434613754107199</v>
       </c>
-      <c r="OX1">
+      <c r="OX1" s="1">
         <v>-0.44633295533469902</v>
       </c>
-      <c r="OY1">
+      <c r="OY1" s="1">
         <v>1.2261881529744201</v>
       </c>
-      <c r="OZ1">
+      <c r="OZ1" s="1">
         <v>0.189574742160908</v>
       </c>
-      <c r="PA1">
+      <c r="PA1" s="1">
         <v>7.5134146943466901E-2</v>
       </c>
-      <c r="PB1">
+      <c r="PB1" s="1">
         <v>0.50322974711419299</v>
       </c>
-      <c r="PC1">
+      <c r="PC1" s="1">
         <v>0.29565211173699901</v>
       </c>
-      <c r="PD1">
+      <c r="PD1" s="1">
         <v>-0.49037815764582898</v>
       </c>
-      <c r="PE1">
+      <c r="PE1" s="1">
         <v>0.752328536067432</v>
       </c>
-      <c r="PF1">
+      <c r="PF1" s="1">
         <v>0.28797664978091297</v>
       </c>
-      <c r="PG1">
+      <c r="PG1" s="1">
         <v>0.28311969295850697</v>
       </c>
-      <c r="PH1">
+      <c r="PH1" s="1">
         <v>-0.221079474733092</v>
       </c>
-      <c r="PI1">
+      <c r="PI1" s="1">
         <v>-0.59902131030539696</v>
       </c>
-      <c r="PJ1">
+      <c r="PJ1" s="1">
         <v>-1.2611294400922199</v>
       </c>
-      <c r="PK1">
+      <c r="PK1" s="1">
         <v>0.324706241385401</v>
       </c>
-      <c r="PL1">
+      <c r="PL1" s="1">
         <v>-0.24215050410118699</v>
       </c>
-      <c r="PM1">
+      <c r="PM1" s="1">
         <v>0.51397562950461795</v>
       </c>
-      <c r="PN1">
+      <c r="PN1" s="1">
         <v>-0.474047335375891</v>
       </c>
-      <c r="PO1">
+      <c r="PO1" s="1">
         <v>0.81706198526503104</v>
       </c>
-      <c r="PP1">
+      <c r="PP1" s="1">
         <v>0.129276456727555</v>
       </c>
-      <c r="PQ1">
+      <c r="PQ1" s="1">
         <v>0.70321095140998202</v>
       </c>
-      <c r="PR1">
+      <c r="PR1" s="1">
         <v>-1.8378116829344801E-2</v>
       </c>
-      <c r="PS1">
+      <c r="PS1" s="1">
         <v>-0.20517178200695399</v>
       </c>
-      <c r="PT1">
+      <c r="PT1" s="1">
         <v>-0.54912657058534398</v>
       </c>
-      <c r="PU1">
+      <c r="PU1" s="1">
         <v>-6.3766084798357006E-2</v>
       </c>
-      <c r="PV1">
+      <c r="PV1" s="1">
         <v>-0.162143321151207</v>
       </c>
-      <c r="PW1">
+      <c r="PW1" s="1">
         <v>-0.418505840775028</v>
       </c>
-      <c r="PX1">
+      <c r="PX1" s="1">
         <v>0.64330902560588199</v>
       </c>
-      <c r="PY1">
+      <c r="PY1" s="1">
         <v>0.74230002050281996</v>
       </c>
-      <c r="PZ1">
+      <c r="PZ1" s="1">
         <v>-0.238333092315722</v>
       </c>
-      <c r="QA1">
+      <c r="QA1" s="1">
         <v>0.37187601973027201</v>
       </c>
-      <c r="QB1">
+      <c r="QB1" s="1">
         <v>-0.80154232190538</v>
       </c>
-      <c r="QC1">
+      <c r="QC1" s="1">
         <v>-0.54728171130728298</v>
       </c>
-      <c r="QD1">
+      <c r="QD1" s="1">
         <v>-7.8778202646343901E-2</v>
       </c>
-      <c r="QE1">
+      <c r="QE1" s="1">
         <v>-0.104484984289029</v>
       </c>
-      <c r="QF1">
+      <c r="QF1" s="1">
         <v>-0.82355452131820195</v>
       </c>
-      <c r="QG1">
+      <c r="QG1" s="1">
         <v>-0.17515739544501099</v>
       </c>
-      <c r="QH1">
+      <c r="QH1" s="1">
         <v>0.63168590698331195</v>
       </c>
-      <c r="QI1">
+      <c r="QI1" s="1">
         <v>5.8308306304090202E-2</v>
       </c>
-      <c r="QJ1">
+      <c r="QJ1" s="1">
         <v>-0.21895676331694999</v>
       </c>
-      <c r="QK1">
+      <c r="QK1" s="1">
         <v>-7.3483088552343699E-3</v>
       </c>
-      <c r="QL1">
+      <c r="QL1" s="1">
         <v>-0.708075779638488</v>
       </c>
-      <c r="QM1">
+      <c r="QM1" s="1">
         <v>-0.51143300843609196</v>
       </c>
-      <c r="QN1">
+      <c r="QN1" s="1">
         <v>1.1037642259568201</v>
       </c>
-      <c r="QO1">
+      <c r="QO1" s="1">
         <v>-0.65296518277653204</v>
       </c>
-      <c r="QP1">
+      <c r="QP1" s="1">
         <v>0.98319524531612401</v>
       </c>
-      <c r="QQ1">
+      <c r="QQ1" s="1">
         <v>-0.50968539216131203</v>
       </c>
-      <c r="QR1">
+      <c r="QR1" s="1">
         <v>-0.15714438546392101</v>
       </c>
-      <c r="QS1">
+      <c r="QS1" s="1">
         <v>0.383556009309589</v>
       </c>
-      <c r="QT1">
+      <c r="QT1" s="1">
         <v>-9.0454540547631704E-2</v>
       </c>
-      <c r="QU1">
+      <c r="QU1" s="1">
         <v>0.375063093322481</v>
       </c>
-      <c r="QV1">
+      <c r="QV1" s="1">
         <v>0.19862922714332901</v>
       </c>
-      <c r="QW1">
+      <c r="QW1" s="1">
         <v>-0.15303881647793699</v>
       </c>
-      <c r="QX1">
+      <c r="QX1" s="1">
         <v>-0.23150060550541399</v>
       </c>
-      <c r="QY1">
+      <c r="QY1" s="1">
         <v>-2.1897979354275499E-2</v>
       </c>
-      <c r="QZ1">
+      <c r="QZ1" s="1">
         <v>-0.32966135679529701</v>
       </c>
-      <c r="RA1">
+      <c r="RA1" s="1">
         <v>0.60863517180619997</v>
       </c>
-      <c r="RB1">
+      <c r="RB1" s="1">
         <v>8.59611867186858E-2</v>
       </c>
-      <c r="RC1">
+      <c r="RC1" s="1">
         <v>-0.46325161232103701</v>
       </c>
-      <c r="RD1">
+      <c r="RD1" s="1">
         <v>0.36276854457867203</v>
       </c>
-      <c r="RE1">
+      <c r="RE1" s="1">
         <v>-0.41683705589166398</v>
       </c>
-      <c r="RF1">
+      <c r="RF1" s="1">
         <v>-0.24085822769364401</v>
       </c>
-      <c r="RG1">
+      <c r="RG1" s="1">
         <v>-0.37833855568053298</v>
       </c>
-      <c r="RH1">
+      <c r="RH1" s="1">
         <v>4.7387635668020303E-2</v>
       </c>
-      <c r="RI1">
+      <c r="RI1" s="1">
         <v>0.32727637362212098</v>
       </c>
-      <c r="RJ1">
+      <c r="RJ1" s="1">
         <v>0.49230535048798402</v>
       </c>
-      <c r="RK1">
+      <c r="RK1" s="1">
         <v>0.226287871804083</v>
       </c>
-      <c r="RL1">
+      <c r="RL1" s="1">
         <v>-0.309492660472867</v>
       </c>
-      <c r="RM1">
+      <c r="RM1" s="1">
         <v>0.46462677175459099</v>
       </c>
-      <c r="RN1">
+      <c r="RN1" s="1">
         <v>-0.62668957953292403</v>
       </c>
-      <c r="RO1">
+      <c r="RO1" s="1">
         <v>-0.76079074519939005</v>
       </c>
-      <c r="RP1">
+      <c r="RP1" s="1">
         <v>0.178623513251393</v>
       </c>
-      <c r="RQ1">
+      <c r="RQ1" s="1">
         <v>0.53759156754375403</v>
       </c>
-      <c r="RR1">
+      <c r="RR1" s="1">
         <v>-0.11713734010210899</v>
       </c>
-      <c r="RS1">
+      <c r="RS1" s="1">
         <v>0.29187038121051301</v>
       </c>
-      <c r="RT1">
+      <c r="RT1" s="1">
         <v>0.195957401014653</v>
       </c>
-      <c r="RU1">
+      <c r="RU1" s="1">
         <v>2.66471113943407E-2</v>
       </c>
-      <c r="RV1">
+      <c r="RV1" s="1">
         <v>-0.37398142928394501</v>
       </c>
-      <c r="RW1">
+      <c r="RW1" s="1">
         <v>-0.12203723905201</v>
       </c>
-      <c r="RX1">
+      <c r="RX1" s="1">
         <v>-0.41209215676240302</v>
       </c>
-      <c r="RY1">
+      <c r="RY1" s="1">
         <v>0.18398084689108499</v>
       </c>
-      <c r="RZ1">
+      <c r="RZ1" s="1">
         <v>0.35887733160063001</v>
       </c>
-      <c r="SA1">
+      <c r="SA1" s="1">
         <v>0.57171767100428905</v>
       </c>
-      <c r="SB1">
+      <c r="SB1" s="1">
         <v>-0.26028925029445099</v>
       </c>
-      <c r="SC1">
+      <c r="SC1" s="1">
         <v>0.337715387957988</v>
       </c>
-      <c r="SD1">
+      <c r="SD1" s="1">
         <v>-0.27694543328305898</v>
       </c>
-      <c r="SE1">
+      <c r="SE1" s="1">
         <v>0.36587845097405902</v>
       </c>
-      <c r="SF1">
+      <c r="SF1" s="1">
         <v>0.123477339051691</v>
       </c>
-      <c r="SG1">
+      <c r="SG1" s="1">
         <v>5.1264469035158799E-2</v>
       </c>
-      <c r="SH1">
+      <c r="SH1" s="1">
         <v>-0.25313985306939801</v>
       </c>
-      <c r="SI1">
+      <c r="SI1" s="1">
         <v>0.326105651460325</v>
       </c>
-      <c r="SJ1">
+      <c r="SJ1" s="1">
         <v>0.64327776883375998</v>
       </c>
-      <c r="SK1">
+      <c r="SK1" s="1">
         <v>0.77029119819596303</v>
       </c>
-      <c r="SL1">
+      <c r="SL1" s="1">
         <v>0.28138481746321098</v>
       </c>
-      <c r="SM1">
+      <c r="SM1" s="1">
         <v>0.14435236558533801</v>
       </c>
-      <c r="SN1">
+      <c r="SN1" s="1">
         <v>-0.50972957516348105</v>
       </c>
-      <c r="SO1">
+      <c r="SO1" s="1">
         <v>0.311133163125555</v>
       </c>
-      <c r="SP1">
+      <c r="SP1" s="1">
         <v>0.49947216257952298</v>
       </c>
-      <c r="SQ1">
+      <c r="SQ1" s="1">
         <v>0.54952862461691498</v>
       </c>
-      <c r="SR1">
+      <c r="SR1" s="1">
         <v>-0.140305981717818</v>
       </c>
-      <c r="SS1">
+      <c r="SS1" s="1">
         <v>-0.59405774051555005</v>
       </c>
-      <c r="ST1">
+      <c r="ST1" s="1">
         <v>0.169630927590876</v>
       </c>
-      <c r="SU1">
+      <c r="SU1" s="1">
         <v>-0.77883652983194096</v>
       </c>
-      <c r="SV1">
+      <c r="SV1" s="1">
         <v>-0.39588705603171298</v>
       </c>
-      <c r="SW1">
+      <c r="SW1" s="1">
         <v>-0.61209916887096505</v>
       </c>
-      <c r="SX1">
+      <c r="SX1" s="1">
         <v>0.16641016902702699</v>
       </c>
-      <c r="SY1">
+      <c r="SY1" s="1">
         <v>-6.2005097354069498E-2</v>
       </c>
-      <c r="SZ1">
+      <c r="SZ1" s="1">
         <v>0.57815440699008402</v>
       </c>
-      <c r="TA1">
+      <c r="TA1" s="1">
         <v>-5.2977022608545102E-2</v>
       </c>
-      <c r="TB1">
+      <c r="TB1" s="1">
         <v>-0.358388983173901</v>
       </c>
-      <c r="TC1">
+      <c r="TC1" s="1">
         <v>-3.9793770688045599E-2</v>
       </c>
-      <c r="TD1">
+      <c r="TD1" s="1">
         <v>-2.6540956156684701E-2</v>
       </c>
-      <c r="TE1">
+      <c r="TE1" s="1">
         <v>0.198916709850292</v>
       </c>
-      <c r="TF1">
+      <c r="TF1" s="1">
         <v>0.19696090101809399</v>
       </c>
-      <c r="TG1">
+      <c r="TG1" s="1">
         <v>-0.203919458865084</v>
       </c>
-      <c r="TH1">
+      <c r="TH1" s="1">
         <v>0.13965339342968899</v>
       </c>
-      <c r="TI1">
+      <c r="TI1" s="1">
         <v>-0.31289803871362598</v>
       </c>
-      <c r="TJ1">
+      <c r="TJ1" s="1">
         <v>0.53232777157095101</v>
       </c>
-      <c r="TK1">
+      <c r="TK1" s="1">
         <v>-3.7585620802832599E-2</v>
       </c>
-      <c r="TL1">
+      <c r="TL1" s="1">
         <v>1.47175623422428</v>
       </c>
-      <c r="TM1">
+      <c r="TM1" s="1">
         <v>-0.19297530853624101</v>
       </c>
-      <c r="TN1">
+      <c r="TN1" s="1">
         <v>-0.31527349769838398</v>
       </c>
-      <c r="TO1">
+      <c r="TO1" s="1">
         <v>-2.5636623171564701E-2</v>
       </c>
-      <c r="TP1">
+      <c r="TP1" s="1">
         <v>-0.10936178062601799</v>
       </c>
-      <c r="TQ1">
+      <c r="TQ1" s="1">
         <v>-0.51230984837250104</v>
       </c>
-      <c r="TR1">
+      <c r="TR1" s="1">
         <v>0.78607082359492697</v>
       </c>
-      <c r="TS1">
+      <c r="TS1" s="1">
         <v>-9.9730195091758997E-2</v>
       </c>
-      <c r="TT1">
+      <c r="TT1" s="1">
         <v>-0.49981277974892901</v>
       </c>
-      <c r="TU1">
+      <c r="TU1" s="1">
         <v>0.56569102899269597</v>
       </c>
-      <c r="TV1">
+      <c r="TV1" s="1">
         <v>-0.46325561346937499</v>
       </c>
-      <c r="TW1">
+      <c r="TW1" s="1">
         <v>1.02934423295722</v>
       </c>
-      <c r="TX1">
+      <c r="TX1" s="1">
         <v>-1.0722003125251001</v>
       </c>
-      <c r="TY1">
+      <c r="TY1" s="1">
         <v>0.39630689106996497</v>
       </c>
-      <c r="TZ1">
+      <c r="TZ1" s="1">
         <v>-0.41327115158862798</v>
       </c>
-      <c r="UA1">
+      <c r="UA1" s="1">
         <v>0.14079589315775901</v>
       </c>
-      <c r="UB1">
+      <c r="UB1" s="1">
         <v>-0.55833916769672698</v>
       </c>
-      <c r="UC1">
+      <c r="UC1" s="1">
         <v>-0.27247262903796599</v>
       </c>
-      <c r="UD1">
+      <c r="UD1" s="1">
         <v>0.180750065844102</v>
       </c>
-      <c r="UE1">
+      <c r="UE1" s="1">
         <v>-1.1971490038317399E-2</v>
       </c>
-      <c r="UF1">
+      <c r="UF1" s="1">
         <v>-0.207067602561464</v>
       </c>
-      <c r="UG1">
+      <c r="UG1" s="1">
         <v>0.79225188806734204</v>
       </c>
-      <c r="UH1">
+      <c r="UH1" s="1">
         <v>-0.109815475099885</v>
       </c>
-      <c r="UI1">
+      <c r="UI1" s="1">
         <v>0.75430103849649599</v>
       </c>
-      <c r="UJ1">
+      <c r="UJ1" s="1">
         <v>-0.52150089917278797</v>
       </c>
-      <c r="UK1">
+      <c r="UK1" s="1">
         <v>-0.451067163551513</v>
       </c>
-      <c r="UL1">
+      <c r="UL1" s="1">
         <v>4.7357459663519501E-2</v>
       </c>
-      <c r="UM1">
+      <c r="UM1" s="1">
         <v>-0.49690727068774099</v>
       </c>
-      <c r="UN1">
+      <c r="UN1" s="1">
         <v>-0.14356955139685501</v>
       </c>
-      <c r="UO1">
+      <c r="UO1" s="1">
         <v>-0.69047184917309001</v>
       </c>
-      <c r="UP1">
+      <c r="UP1" s="1">
         <v>-0.13210980566348199</v>
       </c>
-      <c r="UQ1">
+      <c r="UQ1" s="1">
         <v>-0.229394576594492</v>
       </c>
-      <c r="UR1">
+      <c r="UR1" s="1">
         <v>-1.0634888953974799</v>
       </c>
-      <c r="US1">
+      <c r="US1" s="1">
         <v>0.48042473276500802</v>
       </c>
-      <c r="UT1">
+      <c r="UT1" s="1">
         <v>-0.77083530459098604</v>
       </c>
-      <c r="UU1">
+      <c r="UU1" s="1">
         <v>-0.34717142252593203</v>
       </c>
-      <c r="UV1">
+      <c r="UV1" s="1">
         <v>0.58554251405491697</v>
       </c>
-      <c r="UW1">
+      <c r="UW1" s="1">
         <v>0.723133952486953</v>
       </c>
-      <c r="UX1">
+      <c r="UX1" s="1">
         <v>-0.51500135836912397</v>
       </c>
-      <c r="UY1">
+      <c r="UY1" s="1">
         <v>-0.20970559851833101</v>
       </c>
-      <c r="UZ1">
+      <c r="UZ1" s="1">
         <v>-0.21170180245398201</v>
       </c>
-      <c r="VA1">
+      <c r="VA1" s="1">
         <v>0.39744467878427803</v>
       </c>
-      <c r="VB1">
+      <c r="VB1" s="1">
         <v>0.58897686945673</v>
       </c>
-      <c r="VC1">
+      <c r="VC1" s="1">
         <v>-9.9712009166169097E-2</v>
       </c>
-      <c r="VD1">
+      <c r="VD1" s="1">
         <v>-0.60780199408067304</v>
       </c>
-      <c r="VE1">
+      <c r="VE1" s="1">
         <v>-0.22946568557932401</v>
       </c>
-      <c r="VF1">
+      <c r="VF1" s="1">
         <v>-0.77477555741144699</v>
       </c>
-      <c r="VG1">
+      <c r="VG1" s="1">
         <v>-0.103430934476611</v>
       </c>
-      <c r="VH1">
+      <c r="VH1" s="1">
         <v>0.328836149455486</v>
       </c>
-      <c r="VI1">
+      <c r="VI1" s="1">
         <v>-0.22403824234806299</v>
       </c>
-      <c r="VJ1">
+      <c r="VJ1" s="1">
         <v>-6.8896733100499305E-2</v>
       </c>
-      <c r="VK1">
+      <c r="VK1" s="1">
         <v>-0.92637848128258204</v>
       </c>
-      <c r="VL1">
+      <c r="VL1" s="1">
         <v>-0.59710607590440801</v>
       </c>
-      <c r="VM1">
+      <c r="VM1" s="1">
         <v>-0.36853614363856402</v>
       </c>
-      <c r="VN1">
+      <c r="VN1" s="1">
         <v>-0.99986005651017495</v>
       </c>
-      <c r="VO1">
+      <c r="VO1" s="1">
         <v>-0.68500070025943804</v>
       </c>
-      <c r="VP1">
+      <c r="VP1" s="1">
         <v>-0.57530880017073305</v>
       </c>
-      <c r="VQ1">
+      <c r="VQ1" s="1">
         <v>-0.511151892963156</v>
       </c>
-      <c r="VR1">
+      <c r="VR1" s="1">
         <v>5.1402418037678102E-2</v>
       </c>
-      <c r="VS1">
+      <c r="VS1" s="1">
         <v>0.14911003635470901</v>
       </c>
-      <c r="VT1">
+      <c r="VT1" s="1">
         <v>6.0395430277433902E-2</v>
       </c>
-      <c r="VU1">
+      <c r="VU1" s="1">
         <v>-0.39556551287316</v>
       </c>
-      <c r="VV1">
+      <c r="VV1" s="1">
         <v>0.472921940204999</v>
       </c>
-      <c r="VW1">
+      <c r="VW1" s="1">
         <v>-0.22448010546455999</v>
       </c>
-      <c r="VX1">
+      <c r="VX1" s="1">
         <v>-0.275680084638738</v>
       </c>
-      <c r="VY1">
+      <c r="VY1" s="1">
         <v>0.67600313911584198</v>
       </c>
-      <c r="VZ1">
+      <c r="VZ1" s="1">
         <v>0.25123810389804302</v>
       </c>
-      <c r="WA1">
+      <c r="WA1" s="1">
         <v>0.29980227532076897</v>
       </c>
-      <c r="WB1">
+      <c r="WB1" s="1">
         <v>-4.89739003557896E-2</v>
       </c>
-      <c r="WC1">
+      <c r="WC1" s="1">
         <v>0.65180433941845295</v>
       </c>
-      <c r="WD1">
+      <c r="WD1" s="1">
         <v>4.8428872462096002E-3</v>
       </c>
-      <c r="WE1">
+      <c r="WE1" s="1">
         <v>0.64938983900356295</v>
       </c>
-      <c r="WF1">
+      <c r="WF1" s="1">
         <v>-0.48258263942104601</v>
       </c>
-      <c r="WG1">
+      <c r="WG1" s="1">
         <v>0.46990816252797402</v>
       </c>
-      <c r="WH1">
+      <c r="WH1" s="1">
         <v>-0.57434472029871098</v>
       </c>
-      <c r="WI1">
+      <c r="WI1" s="1">
         <v>-0.11705213491039899</v>
       </c>
-      <c r="WJ1">
+      <c r="WJ1" s="1">
         <v>-0.43846980585097001</v>
       </c>
-      <c r="WK1">
+      <c r="WK1" s="1">
         <v>0.25270376728193999</v>
       </c>
-      <c r="WL1">
+      <c r="WL1" s="1">
         <v>0.932782266556613</v>
       </c>
-      <c r="WM1">
+      <c r="WM1" s="1">
         <v>0.64713253086259304</v>
       </c>
-      <c r="WN1">
+      <c r="WN1" s="1">
         <v>0.35565109659204702</v>
       </c>
-      <c r="WO1">
+      <c r="WO1" s="1">
         <v>-0.16444683801651999</v>
       </c>
-      <c r="WP1">
+      <c r="WP1" s="1">
         <v>0.98375688755785295</v>
       </c>
-      <c r="WQ1">
+      <c r="WQ1" s="1">
         <v>5.5369769682103803E-2</v>
       </c>
-      <c r="WR1">
+      <c r="WR1" s="1">
         <v>-2.9183591590159302E-2</v>
       </c>
-      <c r="WS1">
+      <c r="WS1" s="1">
         <v>0.54197775440027796</v>
       </c>
-      <c r="WT1">
+      <c r="WT1" s="1">
         <v>-0.98462957297937603</v>
       </c>
-      <c r="WU1">
+      <c r="WU1" s="1">
         <v>-0.56746242029897898</v>
       </c>
-      <c r="WV1">
+      <c r="WV1" s="1">
         <v>-8.9349913811528098E-2</v>
       </c>
-      <c r="WW1">
+      <c r="WW1" s="1">
         <v>-5.8006978895337298E-2</v>
       </c>
-      <c r="WX1">
+      <c r="WX1" s="1">
         <v>0.29225277895523599</v>
       </c>
-      <c r="WY1">
+      <c r="WY1" s="1">
         <v>6.5458532650220294E-2</v>
       </c>
-      <c r="WZ1">
+      <c r="WZ1" s="1">
         <v>0.31217532649399499</v>
       </c>
-      <c r="XA1">
+      <c r="XA1" s="1">
         <v>0.16650864955261899</v>
       </c>
-      <c r="XB1">
+      <c r="XB1" s="1">
         <v>0.44269298155638998</v>
       </c>
-      <c r="XC1">
+      <c r="XC1" s="1">
         <v>0.38719409111895098</v>
       </c>
-      <c r="XD1">
+      <c r="XD1" s="1">
         <v>-0.13831227889724401</v>
       </c>
-      <c r="XE1">
+      <c r="XE1" s="1">
         <v>-0.31032713738293399</v>
       </c>
-      <c r="XF1">
+      <c r="XF1" s="1">
         <v>-0.70201485831836397</v>
       </c>
-      <c r="XG1">
+      <c r="XG1" s="1">
         <v>0.43243270122363697</v>
       </c>
-      <c r="XH1">
+      <c r="XH1" s="1">
         <v>0.212286058405148</v>
       </c>
-      <c r="XI1">
+      <c r="XI1" s="1">
         <v>-0.27302105491946399</v>
       </c>
-      <c r="XJ1">
+      <c r="XJ1" s="1">
         <v>-0.41981171728141597</v>
       </c>
-      <c r="XK1">
+      <c r="XK1" s="1">
         <v>-0.55400166233099601</v>
       </c>
-      <c r="XL1">
+      <c r="XL1" s="1">
         <v>0.50346803027751796</v>
       </c>
-      <c r="XM1">
+      <c r="XM1" s="1">
         <v>-6.28974913560163E-2</v>
       </c>
-      <c r="XN1">
+      <c r="XN1" s="1">
         <v>-0.42558977809461901</v>
       </c>
-      <c r="XO1">
+      <c r="XO1" s="1">
         <v>0.17504119209643501</v>
       </c>
-      <c r="XP1">
+      <c r="XP1" s="1">
         <v>-0.74639161253782005</v>
       </c>
-      <c r="XQ1">
+      <c r="XQ1" s="1">
         <v>0.28022980395924801</v>
       </c>
-      <c r="XR1">
+      <c r="XR1" s="1">
         <v>-0.507995943755436</v>
       </c>
-      <c r="XS1">
+      <c r="XS1" s="1">
         <v>-0.480989788074417</v>
       </c>
-      <c r="XT1">
+      <c r="XT1" s="1">
         <v>0.484699628692283</v>
       </c>
-      <c r="XU1">
+      <c r="XU1" s="1">
         <v>0.49904432829623502</v>
       </c>
-      <c r="XV1">
+      <c r="XV1" s="1">
         <v>-0.112264227552722</v>
       </c>
-      <c r="XW1">
+      <c r="XW1" s="1">
         <v>-0.54934795214973997</v>
       </c>
-      <c r="XX1">
+      <c r="XX1" s="1">
         <v>-0.54115207752108396</v>
       </c>
-      <c r="XY1">
+      <c r="XY1" s="1">
         <v>8.42425316242503E-2</v>
       </c>
-      <c r="XZ1">
+      <c r="XZ1" s="1">
         <v>0.347644285064096</v>
       </c>
-      <c r="YA1">
+      <c r="YA1" s="1">
         <v>-0.56644403666224297</v>
       </c>
-      <c r="YB1">
+      <c r="YB1" s="1">
         <v>0.66710409436507101</v>
       </c>
-      <c r="YC1">
+      <c r="YC1" s="1">
         <v>0.51847797525862305</v>
       </c>
-      <c r="YD1">
+      <c r="YD1" s="1">
         <v>0.32340143112364</v>
       </c>
-      <c r="YE1">
+      <c r="YE1" s="1">
         <v>-1.04434880750166</v>
       </c>
-      <c r="YF1">
+      <c r="YF1" s="1">
         <v>4.8224877417691998E-2</v>
       </c>
-      <c r="YG1">
+      <c r="YG1" s="1">
         <v>0.73235254029080699</v>
       </c>
-      <c r="YH1">
+      <c r="YH1" s="1">
         <v>0.12561586417998799</v>
       </c>
-      <c r="YI1">
+      <c r="YI1" s="1">
         <v>0.52259869908744205</v>
       </c>
-      <c r="YJ1">
+      <c r="YJ1" s="1">
         <v>-0.53913726492199099</v>
       </c>
-      <c r="YK1">
+      <c r="YK1" s="1">
         <v>6.5088570126358797E-2</v>
       </c>
-      <c r="YL1">
+      <c r="YL1" s="1">
         <v>-5.4479868017676E-2</v>
       </c>
-      <c r="YM1">
+      <c r="YM1" s="1">
         <v>-0.78252964599893804</v>
       </c>
-      <c r="YN1">
+      <c r="YN1" s="1">
         <v>-0.331015884723804</v>
       </c>
-      <c r="YO1">
+      <c r="YO1" s="1">
         <v>0.119446610304299</v>
       </c>
-      <c r="YP1">
+      <c r="YP1" s="1">
         <v>0.30645531774164497</v>
       </c>
-      <c r="YQ1">
+      <c r="YQ1" s="1">
         <v>4.4751688714568097E-2</v>
       </c>
-      <c r="YR1">
+      <c r="YR1" s="1">
         <v>-1.6064461516687E-3</v>
       </c>
-      <c r="YS1">
+      <c r="YS1" s="1">
         <v>-0.55407932896286904</v>
       </c>
-      <c r="YT1">
+      <c r="YT1" s="1">
         <v>0.60719653660350403</v>
       </c>
-      <c r="YU1">
+      <c r="YU1" s="1">
         <v>0.337373109835783</v>
       </c>
-      <c r="YV1">
+      <c r="YV1" s="1">
         <v>3.7702031023672401E-2</v>
       </c>
-      <c r="YW1">
+      <c r="YW1" s="1">
         <v>0.26428497319799898</v>
       </c>
-      <c r="YX1">
+      <c r="YX1" s="1">
         <v>-1.00861095708994</v>
       </c>
-      <c r="YY1">
+      <c r="YY1" s="1">
         <v>-6.78908313299844E-2</v>
       </c>
-      <c r="YZ1">
+      <c r="YZ1" s="1">
         <v>0.80158715211476195</v>
       </c>
-      <c r="ZA1">
+      <c r="ZA1" s="1">
         <v>-0.52445101446865094</v>
       </c>
-      <c r="ZB1">
+      <c r="ZB1" s="1">
         <v>-0.93199324369426195</v>
       </c>
-      <c r="ZC1">
+      <c r="ZC1" s="1">
         <v>-0.361321362457311</v>
       </c>
-      <c r="ZD1">
+      <c r="ZD1" s="1">
         <v>0.60105108369668303</v>
       </c>
-      <c r="ZE1">
+      <c r="ZE1" s="1">
         <v>-0.17977369855390801</v>
       </c>
-      <c r="ZF1">
+      <c r="ZF1" s="1">
         <v>0.33749229447497298</v>
       </c>
-      <c r="ZG1">
+      <c r="ZG1" s="1">
         <v>-0.32159316276955202</v>
       </c>
-      <c r="ZH1">
+      <c r="ZH1" s="1">
         <v>0.76858658903068899</v>
       </c>
-      <c r="ZI1">
+      <c r="ZI1" s="1">
         <v>-0.18861610122683101</v>
       </c>
-      <c r="ZJ1">
+      <c r="ZJ1" s="1">
         <v>3.1664359482167399E-2</v>
       </c>
-      <c r="ZK1">
+      <c r="ZK1" s="1">
         <v>2.6731938192654299E-2</v>
       </c>
-      <c r="ZL1">
+      <c r="ZL1" s="1">
         <v>-0.50746407818274297</v>
       </c>
-      <c r="ZM1">
+      <c r="ZM1" s="1">
         <v>0.831125889666947</v>
       </c>
-      <c r="ZN1">
+      <c r="ZN1" s="1">
         <v>-0.27358701888003101</v>
       </c>
-      <c r="ZO1">
+      <c r="ZO1" s="1">
         <v>-0.101753003414615</v>
       </c>
-      <c r="ZP1">
+      <c r="ZP1" s="1">
         <v>-0.33056896247335199</v>
       </c>
-      <c r="ZQ1">
+      <c r="ZQ1" s="1">
         <v>-0.38826709331477499</v>
       </c>
-      <c r="ZR1">
+      <c r="ZR1" s="1">
         <v>1.31262162881588E-2</v>
       </c>
-      <c r="ZS1">
+      <c r="ZS1" s="1">
         <v>0.31493127860465597</v>
       </c>
-      <c r="ZT1">
+      <c r="ZT1" s="1">
         <v>-0.38007311032928098</v>
       </c>
-      <c r="ZU1">
+      <c r="ZU1" s="1">
         <v>-0.81051596308095597</v>
       </c>
-      <c r="ZV1">
+      <c r="ZV1" s="1">
         <v>-0.23606388262247299</v>
       </c>
-      <c r="ZW1">
+      <c r="ZW1" s="1">
         <v>0.552405466837259</v>
       </c>
-      <c r="ZX1">
+      <c r="ZX1" s="1">
         <v>-0.588111553639452</v>
       </c>
-      <c r="ZY1">
+      <c r="ZY1" s="1">
         <v>-0.67016013668144103</v>
       </c>
-      <c r="ZZ1">
+      <c r="ZZ1" s="1">
         <v>0.662339674659852</v>
       </c>
-      <c r="AAA1">
+      <c r="AAA1" s="1">
         <v>0.184253367152485</v>
       </c>
-      <c r="AAB1">
+      <c r="AAB1" s="1">
         <v>-0.75436971389171104</v>
       </c>
-      <c r="AAC1">
+      <c r="AAC1" s="1">
         <v>0.11668344271195499</v>
       </c>
-      <c r="AAD1">
+      <c r="AAD1" s="1">
         <v>-0.13424605647169499</v>
       </c>
-      <c r="AAE1">
+      <c r="AAE1" s="1">
         <v>-6.86594194064164E-2</v>
       </c>
-      <c r="AAF1">
+      <c r="AAF1" s="1">
         <v>1.1993157112711601</v>
       </c>
-      <c r="AAG1">
+      <c r="AAG1" s="1">
         <v>6.71982982017231E-2</v>
       </c>
-      <c r="AAH1">
+      <c r="AAH1" s="1">
         <v>-0.64843332962863598</v>
       </c>
-      <c r="AAI1">
+      <c r="AAI1" s="1">
         <v>-0.16678838709539101</v>
       </c>
-      <c r="AAJ1">
+      <c r="AAJ1" s="1">
         <v>-0.30052952135032901</v>
       </c>
-      <c r="AAK1">
+      <c r="AAK1" s="1">
         <v>0.45807141731511702</v>
       </c>
-      <c r="AAL1">
+      <c r="AAL1" s="1">
         <v>-9.4446483088716796E-2</v>
       </c>
-      <c r="AAM1">
+      <c r="AAM1" s="1">
         <v>0.25986607491153002</v>
       </c>
-      <c r="AAN1">
+      <c r="AAN1" s="1">
         <v>8.6363180830291708E-3</v>
       </c>
-      <c r="AAO1">
+      <c r="AAO1" s="1">
         <v>-0.66043966193533998</v>
       </c>
-      <c r="AAP1">
+      <c r="AAP1" s="1">
         <v>-6.8673701948780197E-2</v>
       </c>
-      <c r="AAQ1">
+      <c r="AAQ1" s="1">
         <v>9.2498971113253795E-2</v>
       </c>
-      <c r="AAR1">
+      <c r="AAR1" s="1">
         <v>-0.82930614473194597</v>
       </c>
-      <c r="AAS1">
+      <c r="AAS1" s="1">
         <v>0.17582879994286699</v>
       </c>
-      <c r="AAT1">
+      <c r="AAT1" s="1">
         <v>-0.58226968274776902</v>
       </c>
-      <c r="AAU1">
+      <c r="AAU1" s="1">
         <v>0.61986838734848404</v>
       </c>
-      <c r="AAV1">
+      <c r="AAV1" s="1">
         <v>0.45150059526316699</v>
       </c>
-      <c r="AAW1">
+      <c r="AAW1" s="1">
         <v>0.685791740833682</v>
       </c>
-      <c r="AAX1">
+      <c r="AAX1" s="1">
         <v>-0.29853786105477897</v>
       </c>
-      <c r="AAY1">
+      <c r="AAY1" s="1">
         <v>0.125832989173878</v>
       </c>
-      <c r="AAZ1">
+      <c r="AAZ1" s="1">
         <v>-0.41263680435802702</v>
       </c>
-      <c r="ABA1">
+      <c r="ABA1" s="1">
         <v>4.7932984657158499E-2</v>
       </c>
-      <c r="ABB1">
+      <c r="ABB1" s="1">
         <v>-3.7186989464660598E-2</v>
       </c>
-      <c r="ABC1">
+      <c r="ABC1" s="1">
         <v>-0.103296503710867</v>
       </c>
-      <c r="ABD1">
+      <c r="ABD1" s="1">
         <v>-0.24215088730596401</v>
       </c>
-      <c r="ABE1">
+      <c r="ABE1" s="1">
         <v>-0.62892549205446802</v>
       </c>
-      <c r="ABF1">
+      <c r="ABF1" s="1">
         <v>0.32278070039555201</v>
       </c>
-      <c r="ABG1">
+      <c r="ABG1" s="1">
         <v>-0.52904589942418601</v>
       </c>
-      <c r="ABH1">
+      <c r="ABH1" s="1">
         <v>-0.29274585284445598</v>
       </c>
-      <c r="ABI1">
+      <c r="ABI1" s="1">
         <v>0.13238572423289799</v>
       </c>
-      <c r="ABJ1">
+      <c r="ABJ1" s="1">
         <v>-0.838256722226986</v>
       </c>
-      <c r="ABK1">
+      <c r="ABK1" s="1">
         <v>-0.19224819829325401</v>
       </c>
-      <c r="ABL1">
+      <c r="ABL1" s="1">
         <v>-0.456488556135556</v>
       </c>
-      <c r="ABM1">
+      <c r="ABM1" s="1">
         <v>6.5401013755366097E-2</v>
       </c>
-      <c r="ABN1">
+      <c r="ABN1" s="1">
         <v>-0.165942208762729</v>
       </c>
-      <c r="ABO1">
+      <c r="ABO1" s="1">
         <v>-0.331844479485222</v>
       </c>
-      <c r="ABP1">
+      <c r="ABP1" s="1">
         <v>2.9187384729193099E-2</v>
       </c>
-      <c r="ABQ1">
+      <c r="ABQ1" s="1">
         <v>-0.30136534056830999</v>
       </c>
-      <c r="ABR1">
+      <c r="ABR1" s="1">
         <v>-0.184437110882164</v>
       </c>
-      <c r="ABS1">
+      <c r="ABS1" s="1">
         <v>0.20235248343034001</v>
       </c>
-      <c r="ABT1">
+      <c r="ABT1" s="1">
         <v>1.161553354776</v>
       </c>
-      <c r="ABU1">
+      <c r="ABU1" s="1">
         <v>-0.112382370055907</v>
       </c>
-      <c r="ABV1">
+      <c r="ABV1" s="1">
         <v>7.4820609457846604E-2</v>
       </c>
-      <c r="ABW1">
+      <c r="ABW1" s="1">
         <v>-1.5292923581643801E-2</v>
       </c>
-      <c r="ABX1">
+      <c r="ABX1" s="1">
         <v>-0.253502108246414</v>
       </c>
-      <c r="ABY1">
+      <c r="ABY1" s="1">
         <v>2.24305869433317E-2</v>
       </c>
-      <c r="ABZ1">
+      <c r="ABZ1" s="1">
         <v>0.63806858858077398</v>
       </c>
-      <c r="ACA1">
+      <c r="ACA1" s="1">
         <v>-0.351360614109819</v>
       </c>
-      <c r="ACB1">
+      <c r="ACB1" s="1">
         <v>-0.32501487672901302</v>
       </c>
-      <c r="ACC1">
+      <c r="ACC1" s="1">
         <v>0.92437512319234105</v>
       </c>
-      <c r="ACD1">
+      <c r="ACD1" s="1">
         <v>0.44696005362180802</v>
       </c>
-      <c r="ACE1">
+      <c r="ACE1" s="1">
         <v>0.13238472737166901</v>
       </c>
-      <c r="ACF1">
+      <c r="ACF1" s="1">
         <v>0.51766657481635003</v>
       </c>
-      <c r="ACG1">
+      <c r="ACG1" s="1">
         <v>-0.20655406246709601</v>
       </c>
-      <c r="ACH1">
+      <c r="ACH1" s="1">
         <v>-0.17944691433194301</v>
       </c>
-      <c r="ACI1">
+      <c r="ACI1" s="1">
         <v>0.69696070430463597</v>
       </c>
-      <c r="ACJ1">
+      <c r="ACJ1" s="1">
         <v>-0.38159130001702202</v>
       </c>
-      <c r="ACK1">
+      <c r="ACK1" s="1">
         <v>-0.219784613285291</v>
       </c>
-      <c r="ACL1">
+      <c r="ACL1" s="1">
         <v>0.56079442913322497</v>
       </c>
-      <c r="ACM1">
+      <c r="ACM1" s="1">
         <v>0.79087679875301797</v>
       </c>
-      <c r="ACN1">
+      <c r="ACN1" s="1">
         <v>-0.63711656384395898</v>
       </c>
-      <c r="ACO1">
+      <c r="ACO1" s="1">
         <v>1.08472972218782</v>
       </c>
-      <c r="ACP1">
+      <c r="ACP1" s="1">
         <v>0.73233105904195195</v>
       </c>
-      <c r="ACQ1">
+      <c r="ACQ1" s="1">
         <v>-5.81557102163388E-2</v>
       </c>
-      <c r="ACR1">
+      <c r="ACR1" s="1">
         <v>-4.7558611547542998E-2</v>
       </c>
-      <c r="ACS1">
+      <c r="ACS1" s="1">
         <v>7.2791906071478396E-2</v>
       </c>
-      <c r="ACT1">
+      <c r="ACT1" s="1">
         <v>0.429976032060566</v>
       </c>
-      <c r="ACU1">
+      <c r="ACU1" s="1">
         <v>-0.645185822531961</v>
       </c>
-      <c r="ACV1">
+      <c r="ACV1" s="1">
         <v>-0.40331198482033997</v>
       </c>
-      <c r="ACW1">
+      <c r="ACW1" s="1">
         <v>0.28486774802884401</v>
       </c>
-      <c r="ACX1">
+      <c r="ACX1" s="1">
         <v>-0.79982213914814004</v>
       </c>
-      <c r="ACY1">
+      <c r="ACY1" s="1">
         <v>-0.47146424386452501</v>
       </c>
-      <c r="ACZ1">
+      <c r="ACZ1" s="1">
         <v>5.3323355951219897E-2</v>
       </c>
-      <c r="ADA1">
+      <c r="ADA1" s="1">
         <v>0.20994741430703501</v>
       </c>
-      <c r="ADB1">
+      <c r="ADB1" s="1">
         <v>-0.63958741556458198</v>
       </c>
-      <c r="ADC1">
+      <c r="ADC1" s="1">
         <v>-0.45087791761734503</v>
       </c>
-      <c r="ADD1">
+      <c r="ADD1" s="1">
         <v>-0.164231918669073</v>
       </c>
-      <c r="ADE1">
+      <c r="ADE1" s="1">
         <v>-0.36613307781280902</v>
       </c>
-      <c r="ADF1">
+      <c r="ADF1" s="1">
         <v>-0.18696445522699801</v>
       </c>
-      <c r="ADG1">
+      <c r="ADG1" s="1">
         <v>0.259777094930699</v>
       </c>
-      <c r="ADH1">
+      <c r="ADH1" s="1">
         <v>0.68815720640046696</v>
       </c>
-      <c r="ADI1">
+      <c r="ADI1" s="1">
         <v>9.87440709632805E-2</v>
       </c>
-      <c r="ADJ1">
+      <c r="ADJ1" s="1">
         <v>0.66803555075027499</v>
       </c>
-      <c r="ADK1">
+      <c r="ADK1" s="1">
         <v>-6.0794071067159901E-2</v>
       </c>
-      <c r="ADL1">
+      <c r="ADL1" s="1">
         <v>-0.36135538473813</v>
       </c>
-      <c r="ADM1">
+      <c r="ADM1" s="1">
         <v>-0.116233248658629</v>
       </c>
-      <c r="ADN1">
+      <c r="ADN1" s="1">
         <v>0.41918766061456503</v>
       </c>
-      <c r="ADO1">
+      <c r="ADO1" s="1">
         <v>-0.257068748465696</v>
       </c>
-      <c r="ADP1">
+      <c r="ADP1" s="1">
         <v>0.170513648899832</v>
       </c>
-      <c r="ADQ1">
+      <c r="ADQ1" s="1">
         <v>-0.39935968512088099</v>
       </c>
-      <c r="ADR1">
+      <c r="ADR1" s="1">
         <v>0.39837204276999899</v>
       </c>
-      <c r="ADS1">
+      <c r="ADS1" s="1">
         <v>-0.452024053887429</v>
       </c>
-      <c r="ADT1">
+      <c r="ADT1" s="1">
         <v>-0.41982449106265302</v>
       </c>
-      <c r="ADU1">
+      <c r="ADU1" s="1">
         <v>-2.5457831764889902E-2</v>
       </c>
-      <c r="ADV1">
+      <c r="ADV1" s="1">
         <v>0.27531777180638201</v>
       </c>
-      <c r="ADW1">
+      <c r="ADW1" s="1">
         <v>0.39193047433619099</v>
       </c>
-      <c r="ADX1">
+      <c r="ADX1" s="1">
         <v>0.60681133185807901</v>
       </c>
-      <c r="ADY1">
+      <c r="ADY1" s="1">
         <v>-0.39292635638490397</v>
       </c>
-      <c r="ADZ1">
+      <c r="ADZ1" s="1">
         <v>-0.54422513543830797</v>
       </c>
-      <c r="AEA1">
+      <c r="AEA1" s="1">
         <v>-0.65998005547934901</v>
       </c>
-      <c r="AEB1">
+      <c r="AEB1" s="1">
         <v>-0.45217827261674198</v>
       </c>
-      <c r="AEC1">
+      <c r="AEC1" s="1">
         <v>0.46521235421268098</v>
       </c>
-      <c r="AED1">
+      <c r="AED1" s="1">
         <v>0.127749405405269</v>
       </c>
-      <c r="AEE1">
+      <c r="AEE1" s="1">
         <v>1.1815198491283001</v>
       </c>
-      <c r="AEF1">
+      <c r="AEF1" s="1">
         <v>0.43068578547919001</v>
       </c>
-      <c r="AEG1">
+      <c r="AEG1" s="1">
         <v>-0.59730194389515101</v>
       </c>
-      <c r="AEH1">
+      <c r="AEH1" s="1">
         <v>0.38267815954740703</v>
       </c>
-      <c r="AEI1">
+      <c r="AEI1" s="1">
         <v>9.2161551371670605E-2</v>
       </c>
-      <c r="AEJ1">
+      <c r="AEJ1" s="1">
         <v>-0.28517694331327298</v>
       </c>
-      <c r="AEK1">
+      <c r="AEK1" s="1">
         <v>-0.17358652043428699</v>
       </c>
-      <c r="AEL1">
+      <c r="AEL1" s="1">
         <v>0.228093566109102</v>
       </c>
-      <c r="AEM1">
+      <c r="AEM1" s="1">
         <v>0.30802607363739698</v>
       </c>
-      <c r="AEN1">
+      <c r="AEN1" s="1">
         <v>0.235398335157426</v>
       </c>
-      <c r="AEO1">
+      <c r="AEO1" s="1">
         <v>0.53554051125968105</v>
       </c>
-      <c r="AEP1">
+      <c r="AEP1" s="1">
         <v>0.308213480213133</v>
       </c>
-      <c r="AEQ1">
+      <c r="AEQ1" s="1">
         <v>0.74528446635611101</v>
       </c>
-      <c r="AER1">
+      <c r="AER1" s="1">
         <v>2.87994116266664E-2</v>
       </c>
-      <c r="AES1">
+      <c r="AES1" s="1">
         <v>-1.2907804094070601</v>
       </c>
-      <c r="AET1">
+      <c r="AET1" s="1">
         <v>0.22662258556194301</v>
       </c>
-      <c r="AEU1">
+      <c r="AEU1" s="1">
         <v>0.25698950677197002</v>
       </c>
-      <c r="AEV1">
+      <c r="AEV1" s="1">
         <v>-0.35705682758340701</v>
       </c>
-      <c r="AEW1">
+      <c r="AEW1" s="1">
         <v>0.139162826553</v>
       </c>
-      <c r="AEX1">
+      <c r="AEX1" s="1">
         <v>-0.37818200389266399</v>
       </c>
-      <c r="AEY1">
+      <c r="AEY1" s="1">
         <v>0.19831206369186499</v>
       </c>
-      <c r="AEZ1">
+      <c r="AEZ1" s="1">
         <v>0.47701782974846202</v>
       </c>
-      <c r="AFA1">
+      <c r="AFA1" s="1">
         <v>-0.197630627072058</v>
       </c>
-      <c r="AFB1">
+      <c r="AFB1" s="1">
         <v>-0.93762968953880799</v>
       </c>
-      <c r="AFC1">
+      <c r="AFC1" s="1">
         <v>2.94841776369026E-2</v>
       </c>
-      <c r="AFD1">
+      <c r="AFD1" s="1">
         <v>-0.40306923555526197</v>
       </c>
-      <c r="AFE1">
+      <c r="AFE1" s="1">
         <v>-0.30244514880982998</v>
       </c>
-      <c r="AFF1">
+      <c r="AFF1" s="1">
         <v>0.27479492939560102</v>
       </c>
-      <c r="AFG1">
+      <c r="AFG1" s="1">
         <v>-0.84097559830651603</v>
       </c>
-      <c r="AFH1">
+      <c r="AFH1" s="1">
         <v>0.36523602521111098</v>
       </c>
-      <c r="AFI1">
+      <c r="AFI1" s="1">
         <v>9.9161751429475295E-2</v>
       </c>
-      <c r="AFJ1">
+      <c r="AFJ1" s="1">
         <v>1.3518414310625799</v>
       </c>
-      <c r="AFK1">
+      <c r="AFK1" s="1">
         <v>-6.2586347531015496E-2</v>
       </c>
-      <c r="AFL1">
+      <c r="AFL1" s="1">
         <v>-5.1465274172402903E-2</v>
       </c>
-      <c r="AFM1">
+      <c r="AFM1" s="1">
         <v>-0.52406741108750898</v>
       </c>
-      <c r="AFN1">
+      <c r="AFN1" s="1">
         <v>0.39799439350773802</v>
       </c>
-      <c r="AFO1">
+      <c r="AFO1" s="1">
         <v>0.469655242113449</v>
       </c>
-      <c r="AFP1">
+      <c r="AFP1" s="1">
         <v>0.23748898642048599</v>
       </c>
-      <c r="AFQ1">
+      <c r="AFQ1" s="1">
         <v>-0.54583754364594295</v>
       </c>
-      <c r="AFR1">
+      <c r="AFR1" s="1">
         <v>-6.2703022019120994E-2</v>
       </c>
-      <c r="AFS1">
+      <c r="AFS1" s="1">
         <v>-6.1834338828217802E-2</v>
       </c>
-      <c r="AFT1">
+      <c r="AFT1" s="1">
         <v>-0.16475316452309399</v>
       </c>
-      <c r="AFU1">
+      <c r="AFU1" s="1">
         <v>-0.17205146750435499</v>
       </c>
-      <c r="AFV1">
+      <c r="AFV1" s="1">
         <v>1.40332312260403E-2</v>
       </c>
-      <c r="AFW1">
+      <c r="AFW1" s="1">
         <v>-0.56787492636915804</v>
       </c>
-      <c r="AFX1">
+      <c r="AFX1" s="1">
         <v>-0.91868746664010803</v>
       </c>
-      <c r="AFY1">
+      <c r="AFY1" s="1">
         <v>-1.17861838024987</v>
       </c>
-      <c r="AFZ1">
+      <c r="AFZ1" s="1">
         <v>0.47437673709107298</v>
       </c>
-      <c r="AGA1">
+      <c r="AGA1" s="1">
         <v>-0.26241972469201402</v>
       </c>
-      <c r="AGB1">
+      <c r="AGB1" s="1">
         <v>-0.59588493292178002</v>
       </c>
-      <c r="AGC1">
+      <c r="AGC1" s="1">
         <v>-9.3444006521868697E-2</v>
       </c>
-      <c r="AGD1">
+      <c r="AGD1" s="1">
         <v>5.5821596751410201E-3</v>
       </c>
-      <c r="AGE1">
+      <c r="AGE1" s="1">
         <v>0.253971589317255</v>
       </c>
-      <c r="AGF1">
+      <c r="AGF1" s="1">
         <v>0.41051972173594098</v>
       </c>
-      <c r="AGG1">
+      <c r="AGG1" s="1">
         <v>0.18661656708492</v>
       </c>
-      <c r="AGH1">
+      <c r="AGH1" s="1">
         <v>-0.228940140737945</v>
       </c>
-      <c r="AGI1">
+      <c r="AGI1" s="1">
         <v>0.42260773132393498</v>
       </c>
-      <c r="AGJ1">
+      <c r="AGJ1" s="1">
         <v>0.17652227219486499</v>
       </c>
-      <c r="AGK1">
+      <c r="AGK1" s="1">
         <v>0.38526525087111702</v>
       </c>
-      <c r="AGL1">
+      <c r="AGL1" s="1">
         <v>0.15421777590153199</v>
       </c>
-      <c r="AGM1">
+      <c r="AGM1" s="1">
         <v>0.209694376678633</v>
       </c>
-      <c r="AGN1">
+      <c r="AGN1" s="1">
         <v>-0.30527531744535003</v>
       </c>
-      <c r="AGO1">
+      <c r="AGO1" s="1">
         <v>0.22683241712573099</v>
       </c>
-      <c r="AGP1">
+      <c r="AGP1" s="1">
         <v>-0.693766300624299</v>
       </c>
-      <c r="AGQ1">
+      <c r="AGQ1" s="1">
         <v>0.69120203081923703</v>
       </c>
-      <c r="AGR1">
+      <c r="AGR1" s="1">
         <v>-0.175647156359719</v>
       </c>
-      <c r="AGS1">
+      <c r="AGS1" s="1">
         <v>0.80638149918994295</v>
       </c>
-      <c r="AGT1">
+      <c r="AGT1" s="1">
         <v>0.98207970362188102</v>
       </c>
-      <c r="AGU1">
+      <c r="AGU1" s="1">
         <v>0.55301533480022402</v>
       </c>
-      <c r="AGV1">
+      <c r="AGV1" s="1">
         <v>0.37124058024914802</v>
       </c>
-      <c r="AGW1">
+      <c r="AGW1" s="1">
         <v>0.379167639634786</v>
       </c>
-      <c r="AGX1">
+      <c r="AGX1" s="1">
         <v>0.21603308685734901</v>
       </c>
-      <c r="AGY1">
+      <c r="AGY1" s="1">
         <v>-8.4771565732744095E-2</v>
       </c>
-      <c r="AGZ1">
+      <c r="AGZ1" s="1">
         <v>0.72439060047313597</v>
       </c>
-      <c r="AHA1">
+      <c r="AHA1" s="1">
         <v>0.30463522593829001</v>
       </c>
-      <c r="AHB1">
+      <c r="AHB1" s="1">
         <v>-0.27787660071535802</v>
       </c>
-      <c r="AHC1">
+      <c r="AHC1" s="1">
         <v>0.31306662708752098</v>
       </c>
-      <c r="AHD1">
+      <c r="AHD1" s="1">
         <v>0.66961271854823301</v>
       </c>
-      <c r="AHE1">
+      <c r="AHE1" s="1">
         <v>0.64312221187230201</v>
       </c>
-      <c r="AHF1">
+      <c r="AHF1" s="1">
         <v>0.22321753879446199</v>
       </c>
-      <c r="AHG1">
+      <c r="AHG1" s="1">
         <v>0.833335211291797</v>
       </c>
-      <c r="AHH1">
+      <c r="AHH1" s="1">
         <v>-2.38985801133762E-2</v>
       </c>
-      <c r="AHI1">
+      <c r="AHI1" s="1">
         <v>0.37434410637389398</v>
       </c>
-      <c r="AHJ1">
+      <c r="AHJ1" s="1">
         <v>0.30445240778307198</v>
       </c>
-      <c r="AHK1">
+      <c r="AHK1" s="1">
         <v>0.36954037221642799</v>
       </c>
-      <c r="AHL1">
+      <c r="AHL1" s="1">
         <v>0.58512878451089101</v>
       </c>
-      <c r="AHM1">
+      <c r="AHM1" s="1">
         <v>-7.6117117914299495E-2</v>
       </c>
-      <c r="AHN1">
+      <c r="AHN1" s="1">
         <v>0.82346486467678903</v>
       </c>
-      <c r="AHO1">
+      <c r="AHO1" s="1">
         <v>-0.202149444414121</v>
       </c>
-      <c r="AHP1">
+      <c r="AHP1" s="1">
         <v>-0.51419193853302203</v>
       </c>
-      <c r="AHQ1">
+      <c r="AHQ1" s="1">
         <v>-0.48812999044528599</v>
       </c>
-      <c r="AHR1">
+      <c r="AHR1" s="1">
         <v>0.53296420594116201</v>
       </c>
-      <c r="AHS1">
+      <c r="AHS1" s="1">
         <v>-0.125570693053769</v>
       </c>
-      <c r="AHT1">
+      <c r="AHT1" s="1">
         <v>-0.55459966921107495</v>
       </c>
-      <c r="AHU1">
+      <c r="AHU1" s="1">
         <v>-0.89854224041416497</v>
       </c>
-      <c r="AHV1">
+      <c r="AHV1" s="1">
         <v>0.78400646501348403</v>
       </c>
-      <c r="AHW1">
+      <c r="AHW1" s="1">
         <v>-0.85000524779963005</v>
       </c>
-      <c r="AHX1">
+      <c r="AHX1" s="1">
         <v>0.274339270131574</v>
       </c>
-      <c r="AHY1">
+      <c r="AHY1" s="1">
         <v>1.20733776164757</v>
       </c>
-      <c r="AHZ1">
+      <c r="AHZ1" s="1">
         <v>0.54595748466730398</v>
       </c>
-      <c r="AIA1">
+      <c r="AIA1" s="1">
         <v>-0.49333126579679798</v>
       </c>
-      <c r="AIB1">
+      <c r="AIB1" s="1">
         <v>0.232555224936315</v>
       </c>
-      <c r="AIC1">
+      <c r="AIC1" s="1">
         <v>0.54909316058092705</v>
       </c>
-      <c r="AID1">
+      <c r="AID1" s="1">
         <v>0.105208694727166</v>
       </c>
-      <c r="AIE1">
+      <c r="AIE1" s="1">
         <v>-0.41262633714038199</v>
       </c>
-      <c r="AIF1">
+      <c r="AIF1" s="1">
         <v>-0.57598367121383398</v>
       </c>
-      <c r="AIG1">
+      <c r="AIG1" s="1">
         <v>0.50452135058403402</v>
       </c>
-      <c r="AIH1">
+      <c r="AIH1" s="1">
         <v>5.6109420994237297E-2</v>
       </c>
-      <c r="AII1">
+      <c r="AII1" s="1">
         <v>-4.8627513445108503E-2</v>
       </c>
-      <c r="AIJ1">
+      <c r="AIJ1" s="1">
         <v>-0.25840134385986602</v>
       </c>
-      <c r="AIK1">
+      <c r="AIK1" s="1">
         <v>1.01636567115113</v>
       </c>
-      <c r="AIL1">
+      <c r="AIL1" s="1">
         <v>0.132366731267374</v>
       </c>
-      <c r="AIM1">
+      <c r="AIM1" s="1">
         <v>-7.4372770327636506E-2</v>
       </c>
-      <c r="AIN1">
+      <c r="AIN1" s="1">
         <v>-9.7887899529905106E-2</v>
       </c>
-      <c r="AIO1">
+      <c r="AIO1" s="1">
         <v>-0.53586049191876794</v>
       </c>
-      <c r="AIP1">
+      <c r="AIP1" s="1">
         <v>-0.63809970230285495</v>
       </c>
-      <c r="AIQ1">
+      <c r="AIQ1" s="1">
         <v>-8.8498144586527799E-3</v>
       </c>
-      <c r="AIR1">
+      <c r="AIR1" s="1">
         <v>-0.45319761480174697</v>
       </c>
-      <c r="AIS1">
+      <c r="AIS1" s="1">
         <v>0.72008728248648302</v>
       </c>
-      <c r="AIT1">
+      <c r="AIT1" s="1">
         <v>-5.9561044570065003E-2</v>
       </c>
-      <c r="AIU1">
+      <c r="AIU1" s="1">
         <v>-0.31054480039766902</v>
       </c>
-      <c r="AIV1">
+      <c r="AIV1" s="1">
         <v>-0.59660628441149899</v>
       </c>
-      <c r="AIW1">
+      <c r="AIW1" s="1">
         <v>0.76421355769116295</v>
       </c>
-      <c r="AIX1">
+      <c r="AIX1" s="1">
         <v>0.65923457887178405</v>
       </c>
-      <c r="AIY1">
+      <c r="AIY1" s="1">
         <v>-0.1214100719793</v>
       </c>
-      <c r="AIZ1">
+      <c r="AIZ1" s="1">
         <v>-0.55405267025122196</v>
       </c>
-      <c r="AJA1">
+      <c r="AJA1" s="1">
         <v>0.387055900748766</v>
       </c>
-      <c r="AJB1">
+      <c r="AJB1" s="1">
         <v>-0.38565176990543498</v>
       </c>
-      <c r="AJC1">
+      <c r="AJC1" s="1">
         <v>-0.28552504111008797</v>
       </c>
-      <c r="AJD1">
+      <c r="AJD1" s="1">
         <v>-0.24583324738613299</v>
       </c>
-      <c r="AJE1">
+      <c r="AJE1" s="1">
         <v>0.64575827691301302</v>
       </c>
-      <c r="AJF1">
+      <c r="AJF1" s="1">
         <v>-0.429239943870246</v>
       </c>
-      <c r="AJG1">
+      <c r="AJG1" s="1">
         <v>0.104941599190604</v>
       </c>
-      <c r="AJH1">
+      <c r="AJH1" s="1">
         <v>7.9334251507612696E-2</v>
       </c>
-      <c r="AJI1">
+      <c r="AJI1" s="1">
         <v>0.68638209049540799</v>
       </c>
-      <c r="AJJ1">
+      <c r="AJJ1" s="1">
         <v>-0.38920885353065199</v>
       </c>
-      <c r="AJK1">
+      <c r="AJK1" s="1">
         <v>0.44195936603920599</v>
       </c>
-      <c r="AJL1">
+      <c r="AJL1" s="1">
         <v>-6.1143578344957601E-2</v>
       </c>
-      <c r="AJM1">
+      <c r="AJM1" s="1">
         <v>-0.44578029453081403</v>
       </c>
-      <c r="AJN1">
+      <c r="AJN1" s="1">
         <v>-0.37947897608416598</v>
       </c>
-      <c r="AJO1">
+      <c r="AJO1" s="1">
         <v>0.54830728426779396</v>
       </c>
-      <c r="AJP1">
+      <c r="AJP1" s="1">
         <v>8.7802014485833094E-2</v>
       </c>
-      <c r="AJQ1">
+      <c r="AJQ1" s="1">
         <v>0.61607585457176595</v>
       </c>
-      <c r="AJR1">
+      <c r="AJR1" s="1">
         <v>0.31632167585198401</v>
       </c>
-      <c r="AJS1">
+      <c r="AJS1" s="1">
         <v>0.18867872097107799</v>
       </c>
-      <c r="AJT1">
+      <c r="AJT1" s="1">
         <v>8.98646662443357E-2</v>
       </c>
-      <c r="AJU1">
+      <c r="AJU1" s="1">
         <v>0.36585618811631798</v>
       </c>
-      <c r="AJV1">
+      <c r="AJV1" s="1">
         <v>0.26273929601608298</v>
       </c>
-      <c r="AJW1">
+      <c r="AJW1" s="1">
         <v>0.25654273511576398</v>
       </c>
-      <c r="AJX1">
+      <c r="AJX1" s="1">
         <v>-0.297356257467844</v>
       </c>
-      <c r="AJY1">
+      <c r="AJY1" s="1">
         <v>0.53820664447879496</v>
       </c>
-      <c r="AJZ1">
+      <c r="AJZ1" s="1">
         <v>-6.3278638675427407E-2</v>
       </c>
-      <c r="AKA1">
+      <c r="AKA1" s="1">
         <v>0.131930949959539</v>
       </c>
-      <c r="AKB1">
+      <c r="AKB1" s="1">
         <v>0.36511703428458703</v>
       </c>
-      <c r="AKC1">
+      <c r="AKC1" s="1">
         <v>-0.22535138534792201</v>
       </c>
-      <c r="AKD1">
+      <c r="AKD1" s="1">
         <v>0.356344895396424</v>
       </c>
-      <c r="AKE1">
+      <c r="AKE1" s="1">
         <v>-0.73572061911520004</v>
       </c>
-      <c r="AKF1">
+      <c r="AKF1" s="1">
         <v>0.111495179802377</v>
       </c>
-      <c r="AKG1">
+      <c r="AKG1" s="1">
         <v>-0.60819176062943703</v>
       </c>
-      <c r="AKH1">
+      <c r="AKH1" s="1">
         <v>-1.3291597154669199</v>
       </c>
-      <c r="AKI1">
+      <c r="AKI1" s="1">
         <v>-9.2851347941905193E-2</v>
       </c>
-      <c r="AKJ1">
+      <c r="AKJ1" s="1">
         <v>0.16066942250307201</v>
       </c>
-      <c r="AKK1">
+      <c r="AKK1" s="1">
         <v>-0.29909232433772598</v>
       </c>
-      <c r="AKL1">
+      <c r="AKL1" s="1">
         <v>-0.48860982991188101</v>
       </c>
-      <c r="AKM1">
+      <c r="AKM1" s="1">
         <v>-0.59215195425028899</v>
       </c>
-      <c r="AKN1">
+      <c r="AKN1" s="1">
         <v>-0.83242678981395002</v>
       </c>
-      <c r="AKO1">
+      <c r="AKO1" s="1">
         <v>-0.73332630841943502</v>
       </c>
-      <c r="AKP1">
+      <c r="AKP1" s="1">
         <v>0.23702624789483101</v>
       </c>
-      <c r="AKQ1">
+      <c r="AKQ1" s="1">
         <v>-0.244376692069875</v>
       </c>
-      <c r="AKR1">
+      <c r="AKR1" s="1">
         <v>0.228425645931259</v>
       </c>
-      <c r="AKS1">
+      <c r="AKS1" s="1">
         <v>-0.127657283146108</v>
       </c>
-      <c r="AKT1">
+      <c r="AKT1" s="1">
         <v>-0.118387776116077</v>
       </c>
-      <c r="AKU1">
+      <c r="AKU1" s="1">
         <v>0.22716704951965</v>
       </c>
-      <c r="AKV1">
+      <c r="AKV1" s="1">
         <v>-0.77655228821717504</v>
       </c>
-      <c r="AKW1">
+      <c r="AKW1" s="1">
         <v>-6.1179225731692599E-2</v>
       </c>
-      <c r="AKX1">
+      <c r="AKX1" s="1">
         <v>-8.6356997264888505E-2</v>
       </c>
-      <c r="AKY1">
+      <c r="AKY1" s="1">
         <v>-0.449874719731022</v>
       </c>
-      <c r="AKZ1">
+      <c r="AKZ1" s="1">
         <v>6.4632320387004005E-2</v>
       </c>
-      <c r="ALA1">
+      <c r="ALA1" s="1">
         <v>-7.5858157536275395E-2</v>
       </c>
-      <c r="ALB1">
+      <c r="ALB1" s="1">
         <v>-1.51122975623457</v>
       </c>
-      <c r="ALC1">
+      <c r="ALC1" s="1">
         <v>0.50725207430963104</v>
       </c>
-      <c r="ALD1">
+      <c r="ALD1" s="1">
         <v>-0.31427411477973199</v>
       </c>
-      <c r="ALE1">
+      <c r="ALE1" s="1">
         <v>5.3791946414439497E-2</v>
       </c>
-      <c r="ALF1">
+      <c r="ALF1" s="1">
         <v>2.1734307340068201E-2</v>
       </c>
-      <c r="ALG1">
+      <c r="ALG1" s="1">
         <v>0.65625416359154598</v>
       </c>
-      <c r="ALH1">
+      <c r="ALH1" s="1">
         <v>0.21664472286512301</v>
       </c>
-      <c r="ALI1">
+      <c r="ALI1" s="1">
         <v>0.28893259370604002</v>
       </c>
-      <c r="ALJ1">
+      <c r="ALJ1" s="1">
         <v>0.26511839006330001</v>
       </c>
-      <c r="ALK1">
+      <c r="ALK1" s="1">
         <v>-0.42328277120209101</v>
       </c>
-      <c r="ALL1">
+      <c r="ALL1" s="1">
         <v>0.59356596046544596</v>
       </c>
     </row>

</xml_diff>